<commit_message>
1) change cmds 0x03,0x05
</commit_message>
<xml_diff>
--- a/doc/PTMS_RDM_Tool_Command.xlsx
+++ b/doc/PTMS_RDM_Tool_Command.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="885" windowWidth="14805" windowHeight="7230"/>
+    <workbookView xWindow="240" yWindow="885" windowWidth="14805" windowHeight="7230" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="V1.0" sheetId="1" r:id="rId1"/>
-    <sheet name="Command Frame Format" sheetId="4" r:id="rId2"/>
+    <sheet name="Readme" sheetId="4" r:id="rId1"/>
+    <sheet name="V1.0" sheetId="1" r:id="rId2"/>
+    <sheet name="Revision" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="105">
   <si>
     <t>Bytes</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -221,115 +222,155 @@
     <t>upload IOT settings</t>
   </si>
   <si>
-    <t>upload tag's data</t>
-  </si>
-  <si>
     <t>tag count</t>
   </si>
   <si>
     <t>Tag_1</t>
   </si>
   <si>
+    <t>upper limit</t>
+  </si>
+  <si>
+    <t>RSSI</t>
+  </si>
+  <si>
+    <t>OC_RSSI</t>
+  </si>
+  <si>
+    <t>UINT8</t>
+  </si>
+  <si>
+    <t>UINT32</t>
+  </si>
+  <si>
+    <t>UINT64</t>
+  </si>
+  <si>
+    <t>INT8</t>
+  </si>
+  <si>
+    <t>current temperature</t>
+  </si>
+  <si>
+    <t>INT16</t>
+  </si>
+  <si>
+    <t>[0,31]</t>
+  </si>
+  <si>
+    <t>Tag_N</t>
+  </si>
+  <si>
+    <t>normally is minus</t>
+  </si>
+  <si>
+    <t>0--&gt;RTU,1---&gt;TCP , others  invalid</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>productkey</t>
+  </si>
+  <si>
+    <t>devicename</t>
+  </si>
+  <si>
+    <t>devicesecret</t>
+  </si>
+  <si>
+    <t>regionid</t>
+  </si>
+  <si>
+    <t>UINT16</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>file name</t>
+  </si>
+  <si>
+    <t>will sending file's parameter</t>
+  </si>
+  <si>
+    <t>Note:All data in ethernet frame is lower byte first</t>
+  </si>
+  <si>
+    <t>UDP Port 2800,using to command communication</t>
+  </si>
+  <si>
+    <t>TCP Port ,RDM is the Server,PC tooling is Client, Server listening in port 2900,using to transfer files</t>
+  </si>
+  <si>
+    <t>Command Header</t>
+  </si>
+  <si>
+    <t>Online check</t>
+  </si>
+  <si>
+    <t>upload tags data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>sid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UID</t>
-  </si>
-  <si>
-    <t>upper limit</t>
-  </si>
-  <si>
-    <t>RSSI</t>
-  </si>
-  <si>
-    <t>OC_RSSI</t>
-  </si>
-  <si>
-    <t>UINT8</t>
-  </si>
-  <si>
-    <t>UINT32</t>
-  </si>
-  <si>
-    <t>UINT64</t>
-  </si>
-  <si>
-    <t>INT8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Changes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.08.04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1% ℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>current temperature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>INT16</t>
-  </si>
-  <si>
-    <t>[0,31]</t>
-  </si>
-  <si>
-    <t>Tag_N</t>
-  </si>
-  <si>
-    <t>Celsius degree</t>
-  </si>
-  <si>
-    <t>actual temperature is this part multiply by 0.1</t>
-  </si>
-  <si>
-    <t>normally is minus</t>
-  </si>
-  <si>
-    <t>0--&gt;RTU,1---&gt;TCP , others  invalid</t>
-  </si>
-  <si>
-    <t>0x04</t>
-  </si>
-  <si>
-    <t>productkey</t>
-  </si>
-  <si>
-    <t>devicename</t>
-  </si>
-  <si>
-    <t>devicesecret</t>
-  </si>
-  <si>
-    <t>regionid</t>
-  </si>
-  <si>
-    <t>reserved1</t>
-  </si>
-  <si>
-    <t>UINT16</t>
-  </si>
-  <si>
-    <t>reserved2</t>
-  </si>
-  <si>
-    <t>0x10</t>
-  </si>
-  <si>
-    <t>file name</t>
-  </si>
-  <si>
-    <t>will sending file's parameter</t>
-  </si>
-  <si>
-    <t>Note:All data in ethernet frame is lower byte first</t>
-  </si>
-  <si>
-    <t>file byte size</t>
-  </si>
-  <si>
-    <t>UDP Port 2800,using to command communication</t>
-  </si>
-  <si>
-    <t>TCP Port ,RDM is the Server,PC tooling is Client, Server listening in port 2900,using to transfer files</t>
-  </si>
-  <si>
-    <t>Command Header</t>
-  </si>
-  <si>
-    <t>Online check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1% ℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -412,7 +453,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,6 +490,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="48">
     <border>
@@ -989,7 +1036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1134,9 +1181,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1152,25 +1196,82 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1179,9 +1280,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1194,62 +1292,25 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1555,10 +1616,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U94"/>
+  <dimension ref="B3:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="47.875" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.75" customWidth="1"/>
+    <col min="5" max="5" width="27.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="59" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="59"/>
+    </row>
+    <row r="5" spans="2:7" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B5" s="119" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+    </row>
+    <row r="6" spans="2:7" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B6" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B7" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="55"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B8" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="58" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B13" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="2:7" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B14" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U92"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="F70" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1577,49 +1743,151 @@
     <col min="12" max="12" width="57.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:21" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="87" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:21" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="87" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+    </row>
+    <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="17"/>
+      <c r="B2" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+    </row>
+    <row r="3" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17"/>
+      <c r="B3" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="113" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="113"/>
+      <c r="H3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A4" s="17"/>
+      <c r="B4" s="87" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="17"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="40">
+        <v>2</v>
+      </c>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="32" t="s">
+        <v>31</v>
+      </c>
       <c r="M5" s="16"/>
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
@@ -1630,23 +1898,23 @@
       <c r="T5" s="16"/>
       <c r="U5" s="16"/>
     </row>
-    <row r="6" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6" s="17"/>
-      <c r="B6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="17"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="30">
+        <v>1</v>
+      </c>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="32"/>
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
@@ -1657,39 +1925,23 @@
       <c r="T6" s="16"/>
       <c r="U6" s="16"/>
     </row>
-    <row r="7" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7" s="17"/>
-      <c r="B7" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="23" t="s">
+      <c r="B7" s="88"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="42">
         <v>1</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="95" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="95"/>
-      <c r="H7" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="26" t="s">
-        <v>4</v>
-      </c>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="32"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
       <c r="O7" s="16"/>
@@ -1702,19 +1954,17 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8" s="17"/>
-      <c r="B8" s="104" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="27"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="32"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
@@ -1727,20 +1977,16 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9" s="17"/>
-      <c r="B9" s="105"/>
-      <c r="C9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="93" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="90" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="50" t="s">
+      <c r="B9" s="88"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="106" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="114" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="39" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="40">
@@ -1749,9 +1995,7 @@
       <c r="I9" s="40"/>
       <c r="J9" s="40"/>
       <c r="K9" s="41"/>
-      <c r="L9" s="32" t="s">
-        <v>31</v>
-      </c>
+      <c r="L9" s="32"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
@@ -1764,12 +2008,12 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10" s="17"/>
-      <c r="B10" s="105"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="51" t="s">
+      <c r="B10" s="88"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="6" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="30">
@@ -1791,15 +2035,15 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A11" s="17"/>
-      <c r="B11" s="105"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="49" t="s">
+      <c r="B11" s="88"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="115"/>
+      <c r="G11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="42">
+      <c r="H11" s="30">
         <v>1</v>
       </c>
       <c r="I11" s="42"/>
@@ -1818,17 +2062,25 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12" s="17"/>
-      <c r="B12" s="105"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="32"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="40">
+        <v>16</v>
+      </c>
+      <c r="I12" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="40"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
@@ -1841,25 +2093,25 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13" s="17"/>
-      <c r="B13" s="105"/>
+      <c r="B13" s="88"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="103" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="96" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="40">
-        <v>2</v>
-      </c>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="32"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="30">
+        <v>16</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="30"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
@@ -1870,23 +2122,27 @@
       <c r="T13" s="16"/>
       <c r="U13" s="16"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="17"/>
-      <c r="B14" s="105"/>
+      <c r="B14" s="88"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="97"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="53"/>
       <c r="G14" s="6" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="H14" s="30">
-        <v>1</v>
-      </c>
-      <c r="I14" s="30"/>
+        <v>32</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>22</v>
+      </c>
       <c r="J14" s="30"/>
       <c r="K14" s="31"/>
-      <c r="L14" s="32"/>
+      <c r="L14" s="32" t="s">
+        <v>23</v>
+      </c>
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
@@ -1897,23 +2153,27 @@
       <c r="T14" s="16"/>
       <c r="U14" s="16"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
-      <c r="B15" s="105"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="30">
-        <v>1</v>
-      </c>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="32"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="37">
+        <v>8</v>
+      </c>
+      <c r="I15" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="37"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="45" t="s">
+        <v>21</v>
+      </c>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
@@ -1926,25 +2186,17 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A16" s="17"/>
-      <c r="B16" s="105"/>
+      <c r="B16" s="88"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="40">
-        <v>16</v>
-      </c>
-      <c r="I16" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="32" t="s">
-        <v>21</v>
-      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="32"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
@@ -1957,25 +2209,29 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17" s="17"/>
-      <c r="B17" s="105"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="30">
-        <v>16</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="32" t="s">
-        <v>21</v>
-      </c>
+      <c r="B17" s="88"/>
+      <c r="C17" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="40">
+        <v>2</v>
+      </c>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="32"/>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
@@ -1986,27 +2242,23 @@
       <c r="T17" s="16"/>
       <c r="U17" s="16"/>
     </row>
-    <row r="18" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A18" s="17"/>
-      <c r="B18" s="105"/>
+      <c r="B18" s="88"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="53"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="117"/>
       <c r="G18" s="6" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="H18" s="30">
-        <v>32</v>
-      </c>
-      <c r="I18" s="30" t="s">
-        <v>22</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I18" s="30"/>
       <c r="J18" s="30"/>
       <c r="K18" s="31"/>
-      <c r="L18" s="32" t="s">
-        <v>23</v>
-      </c>
+      <c r="L18" s="32"/>
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
@@ -2017,27 +2269,23 @@
       <c r="T18" s="16"/>
       <c r="U18" s="16"/>
     </row>
-    <row r="19" spans="1:21" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="17"/>
-      <c r="B19" s="105"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="37">
-        <v>8</v>
-      </c>
-      <c r="I19" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="37"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="45" t="s">
-        <v>21</v>
-      </c>
+      <c r="B19" s="88"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="42">
+        <v>1</v>
+      </c>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="32"/>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
@@ -2048,19 +2296,27 @@
       <c r="T19" s="16"/>
       <c r="U19" s="16"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="17"/>
-      <c r="B20" s="105"/>
+      <c r="B20" s="88"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="32"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="94"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="42">
+        <v>16</v>
+      </c>
+      <c r="I20" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="42"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="32" t="s">
+        <v>48</v>
+      </c>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
@@ -2073,28 +2329,16 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A21" s="17"/>
-      <c r="B21" s="105"/>
-      <c r="C21" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" s="93" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="99" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" s="40">
-        <v>2</v>
-      </c>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="41"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="31"/>
       <c r="L21" s="32"/>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
@@ -2108,20 +2352,24 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A22" s="17"/>
-      <c r="B22" s="105"/>
+      <c r="B22" s="88"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="100"/>
-      <c r="G22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="30">
-        <v>1</v>
-      </c>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="31"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="92" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="114" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="40">
+        <v>2</v>
+      </c>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="41"/>
       <c r="L22" s="32"/>
       <c r="M22" s="16"/>
       <c r="N22" s="16"/>
@@ -2133,22 +2381,22 @@
       <c r="T22" s="16"/>
       <c r="U22" s="16"/>
     </row>
-    <row r="23" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23" s="17"/>
-      <c r="B23" s="105"/>
+      <c r="B23" s="88"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="101"/>
-      <c r="G23" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="42">
+      <c r="D23" s="2"/>
+      <c r="E23" s="93"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="30">
         <v>1</v>
       </c>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="43"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="31"/>
       <c r="L23" s="32"/>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
@@ -2162,25 +2410,21 @@
     </row>
     <row r="24" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="17"/>
-      <c r="B24" s="105"/>
+      <c r="B24" s="88"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="102"/>
-      <c r="F24" s="60"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="115"/>
       <c r="G24" s="14" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="H24" s="42">
-        <v>16</v>
-      </c>
-      <c r="I24" s="42" t="s">
-        <v>22</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I24" s="42"/>
       <c r="J24" s="42"/>
       <c r="K24" s="43"/>
-      <c r="L24" s="32" t="s">
-        <v>48</v>
-      </c>
+      <c r="L24" s="32"/>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
@@ -2191,19 +2435,27 @@
       <c r="T24" s="16"/>
       <c r="U24" s="16"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
-      <c r="B25" s="105"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="32"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="98"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="37">
+        <v>16</v>
+      </c>
+      <c r="I25" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="37"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="45" t="s">
+        <v>47</v>
+      </c>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
@@ -2216,24 +2468,16 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A26" s="17"/>
-      <c r="B26" s="105"/>
+      <c r="B26" s="88"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="93" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="G26" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" s="40">
-        <v>2</v>
-      </c>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="41"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
       <c r="L26" s="32"/>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
@@ -2247,20 +2491,16 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27" s="17"/>
-      <c r="B27" s="105"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="97"/>
-      <c r="G27" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H27" s="30">
-        <v>1</v>
-      </c>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="31"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
       <c r="L27" s="32"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
@@ -2272,22 +2512,30 @@
       <c r="T27" s="16"/>
       <c r="U27" s="16"/>
     </row>
-    <row r="28" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A28" s="17"/>
-      <c r="B28" s="105"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="88"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H28" s="42">
-        <v>1</v>
-      </c>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="43"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="40">
+        <v>2</v>
+      </c>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="41"/>
       <c r="L28" s="32"/>
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
@@ -2299,27 +2547,23 @@
       <c r="T28" s="16"/>
       <c r="U28" s="16"/>
     </row>
-    <row r="29" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A29" s="17"/>
-      <c r="B29" s="105"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H29" s="37">
-        <v>16</v>
-      </c>
-      <c r="I29" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" s="37"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="45" t="s">
-        <v>47</v>
-      </c>
+      <c r="B29" s="88"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="93"/>
+      <c r="F29" s="96"/>
+      <c r="G29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="30">
+        <v>1</v>
+      </c>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="32"/>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
       <c r="O29" s="16"/>
@@ -2332,16 +2576,20 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30" s="17"/>
-      <c r="B30" s="105"/>
+      <c r="B30" s="88"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="97"/>
+      <c r="G30" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" s="42">
+        <v>1</v>
+      </c>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="43"/>
       <c r="L30" s="32"/>
       <c r="M30" s="16"/>
       <c r="N30" s="16"/>
@@ -2355,16 +2603,16 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31" s="17"/>
-      <c r="B31" s="105"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="31"/>
       <c r="L31" s="32"/>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
@@ -2378,17 +2626,13 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32" s="17"/>
-      <c r="B32" s="105"/>
-      <c r="C32" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" s="93" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="90" t="s">
+      <c r="B32" s="88"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="92" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G32" s="39" t="s">
@@ -2400,7 +2644,7 @@
       <c r="I32" s="40"/>
       <c r="J32" s="40"/>
       <c r="K32" s="41"/>
-      <c r="L32" s="32"/>
+      <c r="L32" s="38"/>
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
       <c r="O32" s="16"/>
@@ -2413,11 +2657,11 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A33" s="17"/>
-      <c r="B33" s="105"/>
+      <c r="B33" s="88"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="91"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="96"/>
       <c r="G33" s="6" t="s">
         <v>29</v>
       </c>
@@ -2427,7 +2671,7 @@
       <c r="I33" s="30"/>
       <c r="J33" s="30"/>
       <c r="K33" s="31"/>
-      <c r="L33" s="32"/>
+      <c r="L33" s="38"/>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
       <c r="O33" s="16"/>
@@ -2440,11 +2684,11 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A34" s="17"/>
-      <c r="B34" s="105"/>
+      <c r="B34" s="88"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="92"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="97"/>
       <c r="G34" s="14" t="s">
         <v>27</v>
       </c>
@@ -2454,7 +2698,7 @@
       <c r="I34" s="42"/>
       <c r="J34" s="42"/>
       <c r="K34" s="43"/>
-      <c r="L34" s="32"/>
+      <c r="L34" s="38"/>
       <c r="M34" s="16"/>
       <c r="N34" s="16"/>
       <c r="O34" s="16"/>
@@ -2467,17 +2711,25 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A35" s="17"/>
-      <c r="B35" s="105"/>
+      <c r="B35" s="88"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="35"/>
+      <c r="E35" s="93"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
+      <c r="G35" s="120" t="s">
+        <v>52</v>
+      </c>
+      <c r="H35" s="121">
+        <v>1</v>
+      </c>
+      <c r="I35" s="121" t="s">
+        <v>65</v>
+      </c>
       <c r="J35" s="30"/>
       <c r="K35" s="31"/>
-      <c r="L35" s="32"/>
+      <c r="L35" s="38" t="s">
+        <v>74</v>
+      </c>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
       <c r="O35" s="16"/>
@@ -2488,26 +2740,22 @@
       <c r="T35" s="16"/>
       <c r="U35" s="16"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A36" s="17"/>
-      <c r="B36" s="105"/>
+      <c r="B36" s="88"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="93" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="90" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="H36" s="40">
-        <v>2</v>
-      </c>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="41"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" s="121">
+        <v>1</v>
+      </c>
+      <c r="I36" s="121"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="31"/>
       <c r="L36" s="38"/>
       <c r="M36" s="16"/>
       <c r="N36" s="16"/>
@@ -2519,20 +2767,22 @@
       <c r="T36" s="16"/>
       <c r="U36" s="16"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A37" s="17"/>
-      <c r="B37" s="105"/>
+      <c r="B37" s="88"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="88"/>
-      <c r="F37" s="91"/>
-      <c r="G37" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H37" s="30">
-        <v>1</v>
-      </c>
-      <c r="I37" s="30"/>
+      <c r="E37" s="93"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="120" t="s">
+        <v>56</v>
+      </c>
+      <c r="H37" s="121">
+        <v>2</v>
+      </c>
+      <c r="I37" s="121" t="s">
+        <v>80</v>
+      </c>
       <c r="J37" s="30"/>
       <c r="K37" s="31"/>
       <c r="L37" s="38"/>
@@ -2548,20 +2798,22 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A38" s="17"/>
-      <c r="B38" s="105"/>
+      <c r="B38" s="88"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="88"/>
-      <c r="F38" s="92"/>
-      <c r="G38" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H38" s="42">
-        <v>1</v>
-      </c>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="43"/>
+      <c r="E38" s="93"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="H38" s="122">
+        <v>16</v>
+      </c>
+      <c r="I38" s="122" t="s">
+        <v>57</v>
+      </c>
+      <c r="J38" s="30"/>
+      <c r="K38" s="31"/>
       <c r="L38" s="38"/>
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
@@ -2575,25 +2827,23 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A39" s="17"/>
-      <c r="B39" s="105"/>
+      <c r="B39" s="88"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="88"/>
+      <c r="E39" s="93"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H39" s="30">
-        <v>1</v>
-      </c>
-      <c r="I39" s="30" t="s">
-        <v>68</v>
+      <c r="G39" s="120" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39" s="121">
+        <v>4</v>
+      </c>
+      <c r="I39" s="121" t="s">
+        <v>66</v>
       </c>
       <c r="J39" s="30"/>
       <c r="K39" s="31"/>
-      <c r="L39" s="38" t="s">
-        <v>79</v>
-      </c>
+      <c r="L39" s="38"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
@@ -2606,19 +2856,19 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A40" s="17"/>
-      <c r="B40" s="105"/>
+      <c r="B40" s="88"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="88"/>
+      <c r="E40" s="93"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H40" s="1">
-        <v>16</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>57</v>
+      <c r="G40" s="120" t="s">
+        <v>54</v>
+      </c>
+      <c r="H40" s="121">
+        <v>1</v>
+      </c>
+      <c r="I40" s="121" t="s">
+        <v>65</v>
       </c>
       <c r="J40" s="30"/>
       <c r="K40" s="31"/>
@@ -2633,21 +2883,21 @@
       <c r="T40" s="16"/>
       <c r="U40" s="16"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="17"/>
-      <c r="B41" s="105"/>
+      <c r="B41" s="88"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="88"/>
+      <c r="E41" s="93"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H41" s="30">
-        <v>4</v>
-      </c>
-      <c r="I41" s="30" t="s">
-        <v>69</v>
+      <c r="G41" s="120" t="s">
+        <v>55</v>
+      </c>
+      <c r="H41" s="121">
+        <v>1</v>
+      </c>
+      <c r="I41" s="121" t="s">
+        <v>65</v>
       </c>
       <c r="J41" s="30"/>
       <c r="K41" s="31"/>
@@ -2662,25 +2912,23 @@
       <c r="T41" s="16"/>
       <c r="U41" s="16"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
-      <c r="B42" s="105"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="88"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H42" s="30">
-        <v>1</v>
-      </c>
-      <c r="I42" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="J42" s="30"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="38"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="98"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="123" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" s="124">
+        <v>2</v>
+      </c>
+      <c r="I42" s="124"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="45"/>
       <c r="M42" s="16"/>
       <c r="N42" s="16"/>
       <c r="O42" s="16"/>
@@ -2691,25 +2939,19 @@
       <c r="T42" s="16"/>
       <c r="U42" s="16"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A43" s="17"/>
-      <c r="B43" s="105"/>
+      <c r="B43" s="88"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="88"/>
+      <c r="E43" s="9"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H43" s="30">
-        <v>1</v>
-      </c>
-      <c r="I43" s="30" t="s">
-        <v>68</v>
-      </c>
+      <c r="G43" s="6"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
       <c r="J43" s="30"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="38"/>
+      <c r="K43" s="30"/>
+      <c r="L43" s="32"/>
       <c r="M43" s="16"/>
       <c r="N43" s="16"/>
       <c r="O43" s="16"/>
@@ -2722,23 +2964,17 @@
     </row>
     <row r="44" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A44" s="17"/>
-      <c r="B44" s="105"/>
+      <c r="B44" s="88"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="88"/>
+      <c r="E44" s="9"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H44" s="30">
-        <v>2</v>
-      </c>
-      <c r="I44" s="30" t="s">
-        <v>86</v>
-      </c>
+      <c r="G44" s="6"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
       <c r="J44" s="30"/>
-      <c r="K44" s="31"/>
-      <c r="L44" s="38"/>
+      <c r="K44" s="30"/>
+      <c r="L44" s="32"/>
       <c r="M44" s="16"/>
       <c r="N44" s="16"/>
       <c r="O44" s="16"/>
@@ -2749,25 +2985,31 @@
       <c r="T44" s="16"/>
       <c r="U44" s="16"/>
     </row>
-    <row r="45" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A45" s="17"/>
-      <c r="B45" s="105"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="94"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="H45" s="62">
-        <v>1</v>
-      </c>
-      <c r="I45" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="J45" s="37"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="45"/>
+      <c r="B45" s="88"/>
+      <c r="C45" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="40">
+        <v>2</v>
+      </c>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="41"/>
+      <c r="L45" s="32"/>
       <c r="M45" s="16"/>
       <c r="N45" s="16"/>
       <c r="O45" s="16"/>
@@ -2780,16 +3022,20 @@
     </row>
     <row r="46" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A46" s="17"/>
-      <c r="B46" s="105"/>
+      <c r="B46" s="88"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="30"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="93"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H46" s="30">
+        <v>1</v>
+      </c>
       <c r="I46" s="30"/>
       <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
+      <c r="K46" s="31"/>
       <c r="L46" s="32"/>
       <c r="M46" s="16"/>
       <c r="N46" s="16"/>
@@ -2803,16 +3049,20 @@
     </row>
     <row r="47" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A47" s="17"/>
-      <c r="B47" s="105"/>
+      <c r="B47" s="88"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
+      <c r="E47" s="93"/>
+      <c r="F47" s="97"/>
+      <c r="G47" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H47" s="42">
+        <v>1</v>
+      </c>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42"/>
+      <c r="K47" s="43"/>
       <c r="L47" s="32"/>
       <c r="M47" s="16"/>
       <c r="N47" s="16"/>
@@ -2826,28 +3076,16 @@
     </row>
     <row r="48" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A48" s="17"/>
-      <c r="B48" s="105"/>
-      <c r="C48" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E48" s="93" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48" s="90" t="s">
-        <v>5</v>
-      </c>
-      <c r="G48" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="H48" s="40">
-        <v>2</v>
-      </c>
-      <c r="I48" s="40"/>
-      <c r="J48" s="40"/>
-      <c r="K48" s="41"/>
+      <c r="B48" s="88"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="31"/>
       <c r="L48" s="32"/>
       <c r="M48" s="16"/>
       <c r="N48" s="16"/>
@@ -2861,21 +3099,25 @@
     </row>
     <row r="49" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A49" s="17"/>
-      <c r="B49" s="105"/>
+      <c r="B49" s="88"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="88"/>
-      <c r="F49" s="91"/>
-      <c r="G49" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H49" s="30">
-        <v>1</v>
-      </c>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="31"/>
-      <c r="L49" s="32"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="92" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="H49" s="40">
+        <v>2</v>
+      </c>
+      <c r="I49" s="40"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="41"/>
+      <c r="L49" s="38"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
       <c r="O49" s="16"/>
@@ -2888,21 +3130,21 @@
     </row>
     <row r="50" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A50" s="17"/>
-      <c r="B50" s="105"/>
+      <c r="B50" s="88"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="88"/>
-      <c r="F50" s="92"/>
-      <c r="G50" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H50" s="42">
+      <c r="E50" s="93"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H50" s="30">
         <v>1</v>
       </c>
-      <c r="I50" s="42"/>
-      <c r="J50" s="42"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="32"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30"/>
+      <c r="K50" s="31"/>
+      <c r="L50" s="38"/>
       <c r="M50" s="16"/>
       <c r="N50" s="16"/>
       <c r="O50" s="16"/>
@@ -2915,17 +3157,21 @@
     </row>
     <row r="51" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A51" s="17"/>
-      <c r="B51" s="105"/>
+      <c r="B51" s="88"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="31"/>
-      <c r="L51" s="32"/>
+      <c r="E51" s="93"/>
+      <c r="F51" s="97"/>
+      <c r="G51" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H51" s="42">
+        <v>1</v>
+      </c>
+      <c r="I51" s="42"/>
+      <c r="J51" s="42"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="38"/>
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
       <c r="O51" s="16"/>
@@ -2938,24 +3184,22 @@
     </row>
     <row r="52" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A52" s="17"/>
-      <c r="B52" s="105"/>
+      <c r="B52" s="88"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="93" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" s="90" t="s">
-        <v>5</v>
-      </c>
-      <c r="G52" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="H52" s="40">
-        <v>2</v>
-      </c>
-      <c r="I52" s="40"/>
-      <c r="J52" s="40"/>
-      <c r="K52" s="41"/>
+      <c r="E52" s="93"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H52" s="30">
+        <v>16</v>
+      </c>
+      <c r="I52" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="J52" s="30"/>
+      <c r="K52" s="31"/>
       <c r="L52" s="38"/>
       <c r="M52" s="16"/>
       <c r="N52" s="16"/>
@@ -2969,18 +3213,20 @@
     </row>
     <row r="53" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A53" s="17"/>
-      <c r="B53" s="105"/>
+      <c r="B53" s="88"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="88"/>
-      <c r="F53" s="91"/>
+      <c r="E53" s="93"/>
+      <c r="F53" s="2"/>
       <c r="G53" s="6" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="H53" s="30">
-        <v>1</v>
-      </c>
-      <c r="I53" s="30"/>
+        <v>16</v>
+      </c>
+      <c r="I53" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="J53" s="30"/>
       <c r="K53" s="31"/>
       <c r="L53" s="38"/>
@@ -2996,20 +3242,22 @@
     </row>
     <row r="54" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A54" s="17"/>
-      <c r="B54" s="105"/>
+      <c r="B54" s="88"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="88"/>
-      <c r="F54" s="92"/>
-      <c r="G54" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H54" s="42">
-        <v>1</v>
-      </c>
-      <c r="I54" s="42"/>
-      <c r="J54" s="42"/>
-      <c r="K54" s="43"/>
+      <c r="E54" s="93"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H54" s="30">
+        <v>48</v>
+      </c>
+      <c r="I54" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="J54" s="30"/>
+      <c r="K54" s="31"/>
       <c r="L54" s="38"/>
       <c r="M54" s="16"/>
       <c r="N54" s="16"/>
@@ -3021,25 +3269,25 @@
       <c r="T54" s="16"/>
       <c r="U54" s="16"/>
     </row>
-    <row r="55" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:21" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17"/>
-      <c r="B55" s="105"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="88"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H55" s="30">
+      <c r="B55" s="88"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="98"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="H55" s="62">
         <v>16</v>
       </c>
-      <c r="I55" s="30" t="s">
+      <c r="I55" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="J55" s="30"/>
-      <c r="K55" s="31"/>
-      <c r="L55" s="38"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="44"/>
+      <c r="L55" s="45"/>
       <c r="M55" s="16"/>
       <c r="N55" s="16"/>
       <c r="O55" s="16"/>
@@ -3052,23 +3300,17 @@
     </row>
     <row r="56" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A56" s="17"/>
-      <c r="B56" s="105"/>
+      <c r="B56" s="88"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="88"/>
+      <c r="E56" s="9"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H56" s="30">
-        <v>16</v>
-      </c>
-      <c r="I56" s="30" t="s">
-        <v>57</v>
-      </c>
+      <c r="G56" s="6"/>
+      <c r="H56" s="30"/>
+      <c r="I56" s="30"/>
       <c r="J56" s="30"/>
-      <c r="K56" s="31"/>
-      <c r="L56" s="38"/>
+      <c r="K56" s="30"/>
+      <c r="L56" s="79"/>
       <c r="M56" s="16"/>
       <c r="N56" s="16"/>
       <c r="O56" s="16"/>
@@ -3079,25 +3321,19 @@
       <c r="T56" s="16"/>
       <c r="U56" s="16"/>
     </row>
-    <row r="57" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A57" s="17"/>
-      <c r="B57" s="105"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="88"/>
+      <c r="B57" s="88"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="2"/>
       <c r="F57" s="2"/>
-      <c r="G57" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H57" s="30">
-        <v>48</v>
-      </c>
-      <c r="I57" s="30" t="s">
-        <v>57</v>
-      </c>
+      <c r="G57" s="6"/>
+      <c r="H57" s="30"/>
+      <c r="I57" s="30"/>
       <c r="J57" s="30"/>
-      <c r="K57" s="31"/>
-      <c r="L57" s="38"/>
+      <c r="K57" s="30"/>
+      <c r="L57" s="80"/>
       <c r="M57" s="16"/>
       <c r="N57" s="16"/>
       <c r="O57" s="16"/>
@@ -3108,25 +3344,31 @@
       <c r="T57" s="16"/>
       <c r="U57" s="16"/>
     </row>
-    <row r="58" spans="1:21" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A58" s="17"/>
-      <c r="B58" s="105"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="94"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="H58" s="62">
+      <c r="B58" s="88"/>
+      <c r="C58" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="E58" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="I58" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="J58" s="37"/>
-      <c r="K58" s="44"/>
-      <c r="L58" s="45"/>
+      <c r="F58" s="111" t="s">
+        <v>5</v>
+      </c>
+      <c r="G58" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="H58" s="64">
+        <v>2</v>
+      </c>
+      <c r="I58" s="64"/>
+      <c r="J58" s="64"/>
+      <c r="K58" s="65"/>
+      <c r="L58" s="38"/>
       <c r="M58" s="16"/>
       <c r="N58" s="16"/>
       <c r="O58" s="16"/>
@@ -3137,19 +3379,23 @@
       <c r="T58" s="16"/>
       <c r="U58" s="16"/>
     </row>
-    <row r="59" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A59" s="17"/>
-      <c r="B59" s="105"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="30"/>
+      <c r="B59" s="88"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="90"/>
+      <c r="F59" s="96"/>
+      <c r="G59" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H59" s="30">
+        <v>1</v>
+      </c>
       <c r="I59" s="30"/>
       <c r="J59" s="30"/>
-      <c r="K59" s="30"/>
-      <c r="L59" s="80"/>
+      <c r="K59" s="66"/>
+      <c r="L59" s="38"/>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
       <c r="O59" s="16"/>
@@ -3162,17 +3408,21 @@
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A60" s="17"/>
-      <c r="B60" s="105"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="30"/>
-      <c r="I60" s="30"/>
-      <c r="J60" s="30"/>
-      <c r="K60" s="30"/>
-      <c r="L60" s="81"/>
+      <c r="B60" s="88"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="91"/>
+      <c r="F60" s="112"/>
+      <c r="G60" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="H60" s="68">
+        <v>1</v>
+      </c>
+      <c r="I60" s="68"/>
+      <c r="J60" s="68"/>
+      <c r="K60" s="69"/>
+      <c r="L60" s="38"/>
       <c r="M60" s="16"/>
       <c r="N60" s="16"/>
       <c r="O60" s="16"/>
@@ -3185,28 +3435,16 @@
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A61" s="17"/>
-      <c r="B61" s="105"/>
-      <c r="C61" s="70" t="s">
-        <v>10</v>
-      </c>
-      <c r="D61" s="71" t="s">
-        <v>60</v>
-      </c>
-      <c r="E61" s="106" t="s">
-        <v>16</v>
-      </c>
-      <c r="F61" s="118" t="s">
-        <v>5</v>
-      </c>
-      <c r="G61" s="63" t="s">
-        <v>28</v>
-      </c>
-      <c r="H61" s="64">
-        <v>2</v>
-      </c>
-      <c r="I61" s="64"/>
-      <c r="J61" s="64"/>
-      <c r="K61" s="65"/>
+      <c r="B61" s="88"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="76"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="30"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="31"/>
       <c r="L61" s="38"/>
       <c r="M61" s="16"/>
       <c r="N61" s="16"/>
@@ -3220,20 +3458,24 @@
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A62" s="17"/>
-      <c r="B62" s="105"/>
+      <c r="B62" s="88"/>
       <c r="C62" s="13"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="107"/>
-      <c r="F62" s="91"/>
-      <c r="G62" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H62" s="30">
-        <v>1</v>
-      </c>
-      <c r="I62" s="30"/>
-      <c r="J62" s="30"/>
-      <c r="K62" s="66"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="93" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="G62" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="H62" s="64">
+        <v>2</v>
+      </c>
+      <c r="I62" s="40"/>
+      <c r="J62" s="40"/>
+      <c r="K62" s="41"/>
       <c r="L62" s="38"/>
       <c r="M62" s="16"/>
       <c r="N62" s="16"/>
@@ -3247,20 +3489,20 @@
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A63" s="17"/>
-      <c r="B63" s="105"/>
+      <c r="B63" s="88"/>
       <c r="C63" s="13"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="108"/>
-      <c r="F63" s="119"/>
-      <c r="G63" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="H63" s="68">
+      <c r="E63" s="93"/>
+      <c r="F63" s="96"/>
+      <c r="G63" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H63" s="30">
         <v>1</v>
       </c>
-      <c r="I63" s="68"/>
-      <c r="J63" s="68"/>
-      <c r="K63" s="69"/>
+      <c r="I63" s="30"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="31"/>
       <c r="L63" s="38"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
@@ -3274,16 +3516,20 @@
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A64" s="17"/>
-      <c r="B64" s="105"/>
+      <c r="B64" s="88"/>
       <c r="C64" s="13"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="77"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="6"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="30"/>
-      <c r="J64" s="46"/>
-      <c r="K64" s="31"/>
+      <c r="E64" s="93"/>
+      <c r="F64" s="97"/>
+      <c r="G64" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="H64" s="68">
+        <v>1</v>
+      </c>
+      <c r="I64" s="42"/>
+      <c r="J64" s="42"/>
+      <c r="K64" s="43"/>
       <c r="L64" s="38"/>
       <c r="M64" s="16"/>
       <c r="N64" s="16"/>
@@ -3297,24 +3543,22 @@
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A65" s="17"/>
-      <c r="B65" s="105"/>
+      <c r="B65" s="88"/>
       <c r="C65" s="13"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="88" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="90" t="s">
-        <v>5</v>
-      </c>
-      <c r="G65" s="63" t="s">
-        <v>28</v>
-      </c>
-      <c r="H65" s="64">
-        <v>2</v>
-      </c>
-      <c r="I65" s="40"/>
-      <c r="J65" s="40"/>
-      <c r="K65" s="41"/>
+      <c r="E65" s="93"/>
+      <c r="F65" s="99"/>
+      <c r="G65" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="H65" s="121">
+        <v>1</v>
+      </c>
+      <c r="I65" s="121" t="s">
+        <v>65</v>
+      </c>
+      <c r="J65" s="30"/>
+      <c r="K65" s="31"/>
       <c r="L65" s="38"/>
       <c r="M65" s="16"/>
       <c r="N65" s="16"/>
@@ -3326,20 +3570,22 @@
       <c r="T65" s="16"/>
       <c r="U65" s="16"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A66" s="17"/>
-      <c r="B66" s="105"/>
+      <c r="B66" s="88"/>
       <c r="C66" s="13"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="88"/>
-      <c r="F66" s="91"/>
-      <c r="G66" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H66" s="30">
-        <v>1</v>
-      </c>
-      <c r="I66" s="30"/>
+      <c r="E66" s="93"/>
+      <c r="F66" s="100"/>
+      <c r="G66" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="H66" s="121">
+        <v>3</v>
+      </c>
+      <c r="I66" s="121" t="s">
+        <v>65</v>
+      </c>
       <c r="J66" s="30"/>
       <c r="K66" s="31"/>
       <c r="L66" s="38"/>
@@ -3355,20 +3601,24 @@
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A67" s="17"/>
-      <c r="B67" s="105"/>
+      <c r="B67" s="88"/>
       <c r="C67" s="13"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="88"/>
-      <c r="F67" s="92"/>
-      <c r="G67" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="H67" s="68">
-        <v>1</v>
-      </c>
-      <c r="I67" s="42"/>
-      <c r="J67" s="42"/>
-      <c r="K67" s="43"/>
+      <c r="E67" s="93"/>
+      <c r="F67" s="101" t="s">
+        <v>61</v>
+      </c>
+      <c r="G67" s="120" t="s">
+        <v>92</v>
+      </c>
+      <c r="H67" s="121">
+        <v>8</v>
+      </c>
+      <c r="I67" s="121" t="s">
+        <v>67</v>
+      </c>
+      <c r="J67" s="30"/>
+      <c r="K67" s="31"/>
       <c r="L67" s="38"/>
       <c r="M67" s="16"/>
       <c r="N67" s="16"/>
@@ -3382,19 +3632,19 @@
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A68" s="17"/>
-      <c r="B68" s="105"/>
+      <c r="B68" s="88"/>
       <c r="C68" s="13"/>
       <c r="D68" s="2"/>
-      <c r="E68" s="88"/>
-      <c r="F68" s="109"/>
-      <c r="G68" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H68" s="30">
+      <c r="E68" s="93"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="120" t="s">
+        <v>91</v>
+      </c>
+      <c r="H68" s="121">
         <v>1</v>
       </c>
-      <c r="I68" s="30" t="s">
-        <v>68</v>
+      <c r="I68" s="121" t="s">
+        <v>65</v>
       </c>
       <c r="J68" s="30"/>
       <c r="K68" s="31"/>
@@ -3409,21 +3659,21 @@
       <c r="T68" s="16"/>
       <c r="U68" s="16"/>
     </row>
-    <row r="69" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A69" s="17"/>
-      <c r="B69" s="105"/>
+      <c r="B69" s="88"/>
       <c r="C69" s="13"/>
       <c r="D69" s="2"/>
-      <c r="E69" s="88"/>
-      <c r="F69" s="110"/>
-      <c r="G69" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="H69" s="30">
+      <c r="E69" s="93"/>
+      <c r="F69" s="101"/>
+      <c r="G69" s="120" t="s">
+        <v>62</v>
+      </c>
+      <c r="H69" s="121">
         <v>1</v>
       </c>
-      <c r="I69" s="30" t="s">
-        <v>68</v>
+      <c r="I69" s="121" t="s">
+        <v>65</v>
       </c>
       <c r="J69" s="30"/>
       <c r="K69" s="31"/>
@@ -3438,25 +3688,27 @@
       <c r="T69" s="16"/>
       <c r="U69" s="16"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A70" s="17"/>
-      <c r="B70" s="105"/>
+      <c r="B70" s="88"/>
       <c r="C70" s="13"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="88"/>
-      <c r="F70" s="110"/>
-      <c r="G70" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H70" s="30">
-        <v>2</v>
-      </c>
-      <c r="I70" s="30" t="s">
-        <v>86</v>
+      <c r="E70" s="93"/>
+      <c r="F70" s="101"/>
+      <c r="G70" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="H70" s="121">
+        <v>1</v>
+      </c>
+      <c r="I70" s="121" t="s">
+        <v>68</v>
       </c>
       <c r="J70" s="30"/>
       <c r="K70" s="31"/>
-      <c r="L70" s="38"/>
+      <c r="L70" s="38" t="s">
+        <v>73</v>
+      </c>
       <c r="M70" s="16"/>
       <c r="N70" s="16"/>
       <c r="O70" s="16"/>
@@ -3467,26 +3719,26 @@
       <c r="T70" s="16"/>
       <c r="U70" s="16"/>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A71" s="17"/>
-      <c r="B71" s="105"/>
+      <c r="B71" s="88"/>
       <c r="C71" s="13"/>
       <c r="D71" s="2"/>
-      <c r="E71" s="88"/>
-      <c r="F71" s="111" t="s">
-        <v>62</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H71" s="30">
+      <c r="E71" s="93"/>
+      <c r="F71" s="101"/>
+      <c r="G71" s="120" t="s">
+        <v>64</v>
+      </c>
+      <c r="H71" s="121">
         <v>1</v>
       </c>
-      <c r="I71" s="30" t="s">
-        <v>68</v>
+      <c r="I71" s="121" t="s">
+        <v>65</v>
       </c>
       <c r="J71" s="30"/>
-      <c r="K71" s="31"/>
+      <c r="K71" s="31" t="s">
+        <v>71</v>
+      </c>
       <c r="L71" s="38"/>
       <c r="M71" s="16"/>
       <c r="N71" s="16"/>
@@ -3500,21 +3752,23 @@
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A72" s="17"/>
-      <c r="B72" s="105"/>
+      <c r="B72" s="88"/>
       <c r="C72" s="13"/>
       <c r="D72" s="2"/>
-      <c r="E72" s="88"/>
-      <c r="F72" s="111"/>
-      <c r="G72" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H72" s="30">
-        <v>8</v>
-      </c>
-      <c r="I72" s="30" t="s">
+      <c r="E72" s="93"/>
+      <c r="F72" s="101"/>
+      <c r="G72" s="120" t="s">
+        <v>69</v>
+      </c>
+      <c r="H72" s="122">
+        <v>2</v>
+      </c>
+      <c r="I72" s="122" t="s">
         <v>70</v>
       </c>
-      <c r="J72" s="30"/>
+      <c r="J72" s="46" t="s">
+        <v>99</v>
+      </c>
       <c r="K72" s="31"/>
       <c r="L72" s="38"/>
       <c r="M72" s="16"/>
@@ -3527,23 +3781,21 @@
       <c r="T72" s="16"/>
       <c r="U72" s="16"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A73" s="17"/>
-      <c r="B73" s="105"/>
+      <c r="B73" s="88"/>
       <c r="C73" s="13"/>
       <c r="D73" s="2"/>
-      <c r="E73" s="88"/>
-      <c r="F73" s="111"/>
-      <c r="G73" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H73" s="30">
-        <v>1</v>
-      </c>
-      <c r="I73" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="J73" s="30"/>
+      <c r="E73" s="93"/>
+      <c r="F73" s="101"/>
+      <c r="G73" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="H73" s="122">
+        <v>2</v>
+      </c>
+      <c r="I73" s="122"/>
+      <c r="J73" s="46"/>
       <c r="K73" s="31"/>
       <c r="L73" s="38"/>
       <c r="M73" s="16"/>
@@ -3556,27 +3808,23 @@
       <c r="T73" s="16"/>
       <c r="U73" s="16"/>
     </row>
-    <row r="74" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:21" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="17"/>
-      <c r="B74" s="105"/>
+      <c r="B74" s="88"/>
       <c r="C74" s="13"/>
       <c r="D74" s="2"/>
-      <c r="E74" s="88"/>
-      <c r="F74" s="111"/>
-      <c r="G74" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H74" s="30">
-        <v>1</v>
-      </c>
-      <c r="I74" s="30" t="s">
-        <v>71</v>
-      </c>
+      <c r="E74" s="93"/>
+      <c r="F74" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G74" s="120" t="s">
+        <v>19</v>
+      </c>
+      <c r="H74" s="121"/>
+      <c r="I74" s="121"/>
       <c r="J74" s="30"/>
       <c r="K74" s="31"/>
-      <c r="L74" s="38" t="s">
-        <v>78</v>
-      </c>
+      <c r="L74" s="38"/>
       <c r="M74" s="16"/>
       <c r="N74" s="16"/>
       <c r="O74" s="16"/>
@@ -3587,26 +3835,26 @@
       <c r="T74" s="16"/>
       <c r="U74" s="16"/>
     </row>
-    <row r="75" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A75" s="17"/>
-      <c r="B75" s="105"/>
+      <c r="B75" s="88"/>
       <c r="C75" s="13"/>
       <c r="D75" s="2"/>
-      <c r="E75" s="88"/>
-      <c r="F75" s="111"/>
-      <c r="G75" s="6" t="s">
+      <c r="E75" s="93"/>
+      <c r="F75" s="101" t="s">
+        <v>72</v>
+      </c>
+      <c r="G75" s="120" t="s">
+        <v>92</v>
+      </c>
+      <c r="H75" s="121">
+        <v>8</v>
+      </c>
+      <c r="I75" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="H75" s="30">
-        <v>1</v>
-      </c>
-      <c r="I75" s="30" t="s">
-        <v>68</v>
-      </c>
       <c r="J75" s="30"/>
-      <c r="K75" s="31" t="s">
-        <v>74</v>
-      </c>
+      <c r="K75" s="31"/>
       <c r="L75" s="38"/>
       <c r="M75" s="16"/>
       <c r="N75" s="16"/>
@@ -3618,29 +3866,25 @@
       <c r="T75" s="16"/>
       <c r="U75" s="16"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A76" s="17"/>
-      <c r="B76" s="105"/>
+      <c r="B76" s="88"/>
       <c r="C76" s="13"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="88"/>
-      <c r="F76" s="111"/>
-      <c r="G76" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H76" s="1">
-        <v>2</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J76" s="30" t="s">
-        <v>76</v>
-      </c>
+      <c r="E76" s="93"/>
+      <c r="F76" s="101"/>
+      <c r="G76" s="120" t="s">
+        <v>91</v>
+      </c>
+      <c r="H76" s="121">
+        <v>1</v>
+      </c>
+      <c r="I76" s="121" t="s">
+        <v>65</v>
+      </c>
+      <c r="J76" s="30"/>
       <c r="K76" s="31"/>
-      <c r="L76" s="38" t="s">
-        <v>77</v>
-      </c>
+      <c r="L76" s="38"/>
       <c r="M76" s="16"/>
       <c r="N76" s="16"/>
       <c r="O76" s="16"/>
@@ -3651,20 +3895,22 @@
       <c r="T76" s="16"/>
       <c r="U76" s="16"/>
     </row>
-    <row r="77" spans="1:21" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A77" s="17"/>
-      <c r="B77" s="105"/>
+      <c r="B77" s="88"/>
       <c r="C77" s="13"/>
       <c r="D77" s="2"/>
-      <c r="E77" s="88"/>
-      <c r="F77" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H77" s="30"/>
-      <c r="I77" s="30"/>
+      <c r="E77" s="93"/>
+      <c r="F77" s="101"/>
+      <c r="G77" s="120" t="s">
+        <v>62</v>
+      </c>
+      <c r="H77" s="121">
+        <v>1</v>
+      </c>
+      <c r="I77" s="121" t="s">
+        <v>65</v>
+      </c>
       <c r="J77" s="30"/>
       <c r="K77" s="31"/>
       <c r="L77" s="38"/>
@@ -3680,25 +3926,25 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A78" s="17"/>
-      <c r="B78" s="105"/>
+      <c r="B78" s="88"/>
       <c r="C78" s="13"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="88"/>
-      <c r="F78" s="111" t="s">
-        <v>75</v>
-      </c>
-      <c r="G78" s="6" t="s">
+      <c r="E78" s="93"/>
+      <c r="F78" s="101"/>
+      <c r="G78" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="H78" s="30">
+      <c r="H78" s="121">
         <v>1</v>
       </c>
-      <c r="I78" s="30" t="s">
+      <c r="I78" s="121" t="s">
         <v>68</v>
       </c>
       <c r="J78" s="30"/>
       <c r="K78" s="31"/>
-      <c r="L78" s="38"/>
+      <c r="L78" s="38" t="s">
+        <v>73</v>
+      </c>
       <c r="M78" s="16"/>
       <c r="N78" s="16"/>
       <c r="O78" s="16"/>
@@ -3709,24 +3955,26 @@
       <c r="T78" s="16"/>
       <c r="U78" s="16"/>
     </row>
-    <row r="79" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A79" s="17"/>
-      <c r="B79" s="105"/>
+      <c r="B79" s="88"/>
       <c r="C79" s="13"/>
       <c r="D79" s="2"/>
-      <c r="E79" s="88"/>
-      <c r="F79" s="111"/>
-      <c r="G79" s="6" t="s">
+      <c r="E79" s="93"/>
+      <c r="F79" s="101"/>
+      <c r="G79" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="H79" s="30">
-        <v>8</v>
-      </c>
-      <c r="I79" s="30" t="s">
-        <v>70</v>
+      <c r="H79" s="121">
+        <v>1</v>
+      </c>
+      <c r="I79" s="121" t="s">
+        <v>65</v>
       </c>
       <c r="J79" s="30"/>
-      <c r="K79" s="31"/>
+      <c r="K79" s="31" t="s">
+        <v>71</v>
+      </c>
       <c r="L79" s="38"/>
       <c r="M79" s="16"/>
       <c r="N79" s="16"/>
@@ -3740,21 +3988,23 @@
     </row>
     <row r="80" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A80" s="17"/>
-      <c r="B80" s="105"/>
+      <c r="B80" s="88"/>
       <c r="C80" s="13"/>
       <c r="D80" s="2"/>
-      <c r="E80" s="88"/>
-      <c r="F80" s="111"/>
-      <c r="G80" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H80" s="30">
-        <v>1</v>
-      </c>
-      <c r="I80" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="J80" s="30"/>
+      <c r="E80" s="93"/>
+      <c r="F80" s="101"/>
+      <c r="G80" s="120" t="s">
+        <v>100</v>
+      </c>
+      <c r="H80" s="121">
+        <v>2</v>
+      </c>
+      <c r="I80" s="121" t="s">
+        <v>101</v>
+      </c>
+      <c r="J80" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="K80" s="31"/>
       <c r="L80" s="38"/>
       <c r="M80" s="16"/>
@@ -3767,27 +4017,23 @@
       <c r="T80" s="16"/>
       <c r="U80" s="16"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A81" s="17"/>
-      <c r="B81" s="105"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="88"/>
-      <c r="F81" s="111"/>
-      <c r="G81" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H81" s="30">
-        <v>1</v>
-      </c>
-      <c r="I81" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="J81" s="30"/>
-      <c r="K81" s="31"/>
-      <c r="L81" s="38" t="s">
-        <v>78</v>
-      </c>
+      <c r="B81" s="88"/>
+      <c r="C81" s="72"/>
+      <c r="D81" s="73"/>
+      <c r="E81" s="107"/>
+      <c r="F81" s="102"/>
+      <c r="G81" s="123" t="s">
+        <v>103</v>
+      </c>
+      <c r="H81" s="125">
+        <v>2</v>
+      </c>
+      <c r="I81" s="125"/>
+      <c r="J81" s="62"/>
+      <c r="K81" s="74"/>
+      <c r="L81" s="75"/>
       <c r="M81" s="16"/>
       <c r="N81" s="16"/>
       <c r="O81" s="16"/>
@@ -3799,288 +4045,224 @@
       <c r="U81" s="16"/>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A82" s="17"/>
-      <c r="B82" s="105"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="88"/>
-      <c r="F82" s="111"/>
-      <c r="G82" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H82" s="30">
-        <v>1</v>
-      </c>
-      <c r="I82" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="J82" s="30"/>
-      <c r="K82" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="L82" s="38"/>
-      <c r="M82" s="16"/>
-      <c r="N82" s="16"/>
-      <c r="O82" s="16"/>
-      <c r="P82" s="16"/>
-      <c r="Q82" s="16"/>
-      <c r="R82" s="16"/>
-      <c r="S82" s="16"/>
-      <c r="T82" s="16"/>
-      <c r="U82" s="16"/>
-    </row>
-    <row r="83" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="17"/>
-      <c r="B83" s="105"/>
-      <c r="C83" s="72"/>
-      <c r="D83" s="73"/>
-      <c r="E83" s="89"/>
-      <c r="F83" s="112"/>
-      <c r="G83" s="61" t="s">
-        <v>72</v>
-      </c>
-      <c r="H83" s="76">
+      <c r="B82" s="88"/>
+      <c r="L82" s="77"/>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A83" s="1"/>
+      <c r="B83" s="88"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="L83" s="78"/>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A84" s="1"/>
+      <c r="B84" s="88"/>
+      <c r="C84" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D84" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="E84" s="89" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" s="103" t="s">
+        <v>5</v>
+      </c>
+      <c r="G84" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="H84" s="64">
         <v>2</v>
       </c>
-      <c r="I83" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="J83" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="K83" s="74"/>
-      <c r="L83" s="75" t="s">
-        <v>77</v>
-      </c>
-      <c r="M83" s="16"/>
-      <c r="N83" s="16"/>
-      <c r="O83" s="16"/>
-      <c r="P83" s="16"/>
-      <c r="Q83" s="16"/>
-      <c r="R83" s="16"/>
-      <c r="S83" s="16"/>
-      <c r="T83" s="16"/>
-      <c r="U83" s="16"/>
-    </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="B84" s="105"/>
-      <c r="L84" s="78"/>
+      <c r="I84" s="64"/>
+      <c r="J84" s="64"/>
+      <c r="K84" s="65"/>
+      <c r="L84" s="81"/>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A85" s="1"/>
-      <c r="B85" s="105"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="L85" s="79"/>
+      <c r="B85" s="88"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="90"/>
+      <c r="F85" s="104"/>
+      <c r="G85" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H85" s="30">
+        <v>1</v>
+      </c>
+      <c r="I85" s="30"/>
+      <c r="J85" s="30"/>
+      <c r="K85" s="66"/>
+      <c r="L85" s="38"/>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A86" s="1"/>
-      <c r="B86" s="105"/>
-      <c r="C86" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="D86" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="E86" s="106" t="s">
-        <v>12</v>
-      </c>
-      <c r="F86" s="113" t="s">
-        <v>5</v>
-      </c>
-      <c r="G86" s="63" t="s">
-        <v>28</v>
-      </c>
-      <c r="H86" s="64">
-        <v>2</v>
-      </c>
-      <c r="I86" s="64"/>
-      <c r="J86" s="64"/>
-      <c r="K86" s="65"/>
-      <c r="L86" s="82"/>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="B86" s="88"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="90"/>
+      <c r="F86" s="105"/>
+      <c r="G86" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H86" s="42">
+        <v>1</v>
+      </c>
+      <c r="I86" s="42"/>
+      <c r="J86" s="42"/>
+      <c r="K86" s="82"/>
+      <c r="L86" s="38"/>
+    </row>
+    <row r="87" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A87" s="1"/>
-      <c r="B87" s="105"/>
+      <c r="B87" s="88"/>
       <c r="C87" s="2"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="107"/>
-      <c r="F87" s="114"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="90"/>
+      <c r="F87" s="83"/>
       <c r="G87" s="6" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="H87" s="30">
-        <v>1</v>
-      </c>
-      <c r="I87" s="30"/>
+        <v>4</v>
+      </c>
+      <c r="I87" s="30" t="s">
+        <v>66</v>
+      </c>
       <c r="J87" s="30"/>
       <c r="K87" s="66"/>
       <c r="L87" s="38"/>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A88" s="1"/>
-      <c r="B88" s="105"/>
+      <c r="B88" s="88"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
-      <c r="E88" s="107"/>
-      <c r="F88" s="115"/>
-      <c r="G88" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H88" s="42">
-        <v>1</v>
-      </c>
-      <c r="I88" s="42"/>
-      <c r="J88" s="42"/>
-      <c r="K88" s="83"/>
+      <c r="E88" s="91"/>
+      <c r="F88" s="84"/>
+      <c r="G88" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="H88" s="68">
+        <v>16</v>
+      </c>
+      <c r="I88" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="J88" s="68"/>
+      <c r="K88" s="69"/>
       <c r="L88" s="38"/>
     </row>
-    <row r="89" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A89" s="1"/>
-      <c r="B89" s="105"/>
+      <c r="B89" s="88"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="107"/>
-      <c r="F89" s="84"/>
-      <c r="G89" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H89" s="30">
-        <v>4</v>
-      </c>
-      <c r="I89" s="30" t="s">
-        <v>69</v>
-      </c>
+      <c r="E89" s="76"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="30"/>
+      <c r="I89" s="30"/>
       <c r="J89" s="30"/>
-      <c r="K89" s="66"/>
-      <c r="L89" s="38"/>
-    </row>
-    <row r="90" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="K89" s="31"/>
+      <c r="L89" s="32"/>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A90" s="1"/>
-      <c r="B90" s="105"/>
+      <c r="B90" s="88"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
-      <c r="E90" s="108"/>
-      <c r="F90" s="85"/>
-      <c r="G90" s="67" t="s">
-        <v>89</v>
-      </c>
-      <c r="H90" s="68">
-        <v>16</v>
-      </c>
-      <c r="I90" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="J90" s="68"/>
-      <c r="K90" s="69"/>
+      <c r="E90" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="F90" s="108" t="s">
+        <v>5</v>
+      </c>
+      <c r="G90" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="H90" s="40">
+        <v>2</v>
+      </c>
+      <c r="I90" s="40"/>
+      <c r="J90" s="40"/>
+      <c r="K90" s="41"/>
       <c r="L90" s="38"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A91" s="1"/>
-      <c r="B91" s="105"/>
+      <c r="B91" s="88"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
-      <c r="E91" s="77"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="6"/>
-      <c r="H91" s="30"/>
+      <c r="E91" s="93"/>
+      <c r="F91" s="109"/>
+      <c r="G91" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H91" s="30">
+        <v>1</v>
+      </c>
       <c r="I91" s="30"/>
       <c r="J91" s="30"/>
       <c r="K91" s="31"/>
-      <c r="L91" s="32"/>
-    </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="L91" s="38"/>
+    </row>
+    <row r="92" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
-      <c r="B92" s="105"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="103" t="s">
-        <v>13</v>
-      </c>
-      <c r="F92" s="116" t="s">
-        <v>5</v>
-      </c>
-      <c r="G92" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="H92" s="40">
-        <v>2</v>
-      </c>
-      <c r="I92" s="40"/>
-      <c r="J92" s="40"/>
-      <c r="K92" s="41"/>
-      <c r="L92" s="38"/>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A93" s="1"/>
-      <c r="B93" s="105"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="88"/>
-      <c r="F93" s="97"/>
-      <c r="G93" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H93" s="30">
+      <c r="B92" s="88"/>
+      <c r="C92" s="73"/>
+      <c r="D92" s="85"/>
+      <c r="E92" s="107"/>
+      <c r="F92" s="110"/>
+      <c r="G92" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="H92" s="62">
         <v>1</v>
       </c>
-      <c r="I93" s="30"/>
-      <c r="J93" s="30"/>
-      <c r="K93" s="31"/>
-      <c r="L93" s="38"/>
-    </row>
-    <row r="94" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="1"/>
-      <c r="B94" s="105"/>
-      <c r="C94" s="73"/>
-      <c r="D94" s="86"/>
-      <c r="E94" s="89"/>
-      <c r="F94" s="117"/>
-      <c r="G94" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="H94" s="62">
-        <v>1</v>
-      </c>
-      <c r="I94" s="62"/>
-      <c r="J94" s="62"/>
-      <c r="K94" s="74"/>
-      <c r="L94" s="75"/>
+      <c r="I92" s="62"/>
+      <c r="J92" s="62"/>
+      <c r="K92" s="74"/>
+      <c r="L92" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B8:B94"/>
-    <mergeCell ref="E86:E90"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="E48:E50"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="E52:E58"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="F68:F70"/>
-    <mergeCell ref="F71:F76"/>
-    <mergeCell ref="F78:F83"/>
-    <mergeCell ref="E61:E63"/>
-    <mergeCell ref="F86:F88"/>
-    <mergeCell ref="E92:E94"/>
-    <mergeCell ref="F92:F94"/>
-    <mergeCell ref="F61:F63"/>
+    <mergeCell ref="E62:E81"/>
+    <mergeCell ref="F62:F64"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="E32:E42"/>
     <mergeCell ref="F32:F34"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F67:F73"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="E9:E15"/>
     <mergeCell ref="F9:F11"/>
-    <mergeCell ref="E13:E19"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="E65:E83"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="E36:E45"/>
-    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="B4:B92"/>
+    <mergeCell ref="E84:E88"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="E49:E55"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="F75:F81"/>
+    <mergeCell ref="E58:E60"/>
+    <mergeCell ref="F84:F86"/>
+    <mergeCell ref="E90:E92"/>
+    <mergeCell ref="F90:F92"/>
+    <mergeCell ref="F58:F60"/>
+    <mergeCell ref="F28:F30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4088,82 +4270,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H3:K10"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.75" customWidth="1"/>
-    <col min="11" max="11" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="8:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="H3" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="8:11" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="H4" s="59"/>
-    </row>
-    <row r="5" spans="8:11" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="H5" s="120" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="126" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-    </row>
-    <row r="6" spans="8:11" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="H6" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="56" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="57" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="8:11" x14ac:dyDescent="0.15">
-      <c r="H7" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="55"/>
-    </row>
-    <row r="8" spans="8:11" x14ac:dyDescent="0.15">
-      <c r="H8" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="55" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="8:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H10" s="58" t="s">
-        <v>91</v>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="126" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H5:J5"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1) get online tags to gui is ok 2) edit in tableview is ok
</commit_message>
<xml_diff>
--- a/doc/PTMS_RDM_Tool_Command.xlsx
+++ b/doc/PTMS_RDM_Tool_Command.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
-    <sheet name="V1.1" sheetId="1" r:id="rId2"/>
+    <sheet name="V1.2" sheetId="1" r:id="rId2"/>
     <sheet name="Revision" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="142">
   <si>
     <t>Bytes</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -344,10 +344,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>reserved</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>file size</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -400,10 +396,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>note</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -517,6 +509,18 @@
   </si>
   <si>
     <t>upload managed-tags settings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.08.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>change cmd 0x7: add tag name and note in command</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1331,9 +1335,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1341,127 +1342,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1471,15 +1356,134 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1807,11 +1811,11 @@
       <c r="B4" s="59"/>
     </row>
     <row r="5" spans="2:7" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="97" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
     </row>
     <row r="6" spans="2:7" ht="14.25" x14ac:dyDescent="0.15">
       <c r="B6" s="56" t="s">
@@ -1886,13 +1890,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U161"/>
+  <dimension ref="A1:U165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D78" sqref="D78"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1903,9 +1907,9 @@
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.75" customWidth="1"/>
-    <col min="7" max="7" width="28.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28.25" style="138" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.75" style="136" customWidth="1"/>
+    <col min="9" max="9" width="12" style="136" customWidth="1"/>
     <col min="10" max="10" width="20" style="1" customWidth="1"/>
     <col min="11" max="11" width="11.25" style="1" customWidth="1"/>
     <col min="12" max="12" width="57.125" customWidth="1"/>
@@ -1918,9 +1922,9 @@
       <c r="D1" s="18"/>
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
       <c r="L1" s="17"/>
@@ -1940,14 +1944,14 @@
         <v>14</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
       <c r="L2" s="17"/>
@@ -1975,14 +1979,14 @@
       <c r="E3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="97"/>
-      <c r="H3" s="24" t="s">
+      <c r="G3" s="129"/>
+      <c r="H3" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="135" t="s">
         <v>8</v>
       </c>
       <c r="J3" s="24" t="s">
@@ -2006,16 +2010,16 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A4" s="17"/>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="111" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
       <c r="J4" s="4"/>
       <c r="K4" s="5"/>
       <c r="L4" s="27"/>
@@ -2031,17 +2035,17 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5" s="17"/>
-      <c r="B5" s="107"/>
+      <c r="B5" s="112"/>
       <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" s="94" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="91" t="s">
+      <c r="F5" s="100" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="50" t="s">
@@ -2068,11 +2072,11 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6" s="17"/>
-      <c r="B6" s="107"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="17"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="92"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="101"/>
       <c r="G6" s="51" t="s">
         <v>26</v>
       </c>
@@ -2095,11 +2099,11 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7" s="17"/>
-      <c r="B7" s="107"/>
+      <c r="B7" s="112"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="93"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="102"/>
       <c r="G7" s="49" t="s">
         <v>24</v>
       </c>
@@ -2122,7 +2126,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8" s="17"/>
-      <c r="B8" s="107"/>
+      <c r="B8" s="112"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -2145,13 +2149,13 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9" s="17"/>
-      <c r="B9" s="107"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="105" t="s">
+      <c r="E9" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="98" t="s">
+      <c r="F9" s="106" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="39" t="s">
@@ -2176,11 +2180,11 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10" s="17"/>
-      <c r="B10" s="107"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="99"/>
+      <c r="E10" s="99"/>
+      <c r="F10" s="107"/>
       <c r="G10" s="6" t="s">
         <v>26</v>
       </c>
@@ -2203,11 +2207,11 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A11" s="17"/>
-      <c r="B11" s="107"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="100"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="108"/>
       <c r="G11" s="6" t="s">
         <v>24</v>
       </c>
@@ -2230,10 +2234,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12" s="17"/>
-      <c r="B12" s="107"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="89"/>
+      <c r="E12" s="99"/>
       <c r="F12" s="52"/>
       <c r="G12" s="39" t="s">
         <v>38</v>
@@ -2261,10 +2265,10 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13" s="17"/>
-      <c r="B13" s="107"/>
+      <c r="B13" s="112"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="89"/>
+      <c r="E13" s="99"/>
       <c r="F13" s="53"/>
       <c r="G13" s="6" t="s">
         <v>40</v>
@@ -2292,10 +2296,10 @@
     </row>
     <row r="14" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="17"/>
-      <c r="B14" s="107"/>
+      <c r="B14" s="112"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="89"/>
+      <c r="E14" s="99"/>
       <c r="F14" s="53"/>
       <c r="G14" s="6" t="s">
         <v>41</v>
@@ -2323,19 +2327,19 @@
     </row>
     <row r="15" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="17"/>
-      <c r="B15" s="107"/>
+      <c r="B15" s="112"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="89"/>
+      <c r="E15" s="99"/>
       <c r="F15" s="29"/>
       <c r="G15" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H15" s="30">
         <v>8</v>
       </c>
       <c r="I15" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J15" s="30"/>
       <c r="K15" s="31"/>
@@ -2354,22 +2358,22 @@
     </row>
     <row r="16" spans="1:21" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
-      <c r="B16" s="107"/>
+      <c r="B16" s="112"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="90"/>
+      <c r="E16" s="125"/>
       <c r="F16" s="33"/>
-      <c r="G16" s="125" t="s">
-        <v>132</v>
-      </c>
-      <c r="H16" s="137">
+      <c r="G16" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="H16" s="37">
         <v>16</v>
       </c>
-      <c r="I16" s="137" t="s">
+      <c r="I16" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="137"/>
-      <c r="K16" s="138"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="96"/>
       <c r="L16" s="45" t="s">
         <v>19</v>
       </c>
@@ -2385,11 +2389,11 @@
     </row>
     <row r="17" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="17"/>
-      <c r="B17" s="107"/>
+      <c r="B17" s="112"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="130"/>
+      <c r="F17" s="89"/>
       <c r="G17" s="6"/>
       <c r="H17" s="30"/>
       <c r="I17" s="30"/>
@@ -2408,7 +2412,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A18" s="17"/>
-      <c r="B18" s="107"/>
+      <c r="B18" s="112"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -2431,17 +2435,17 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A19" s="17"/>
-      <c r="B19" s="107"/>
+      <c r="B19" s="112"/>
       <c r="C19" s="34" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="94" t="s">
+      <c r="E19" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="101" t="s">
+      <c r="F19" s="130" t="s">
         <v>5</v>
       </c>
       <c r="G19" s="39" t="s">
@@ -2466,11 +2470,11 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20" s="17"/>
-      <c r="B20" s="107"/>
+      <c r="B20" s="112"/>
       <c r="C20" s="2"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="102"/>
+      <c r="E20" s="99"/>
+      <c r="F20" s="131"/>
       <c r="G20" s="6" t="s">
         <v>26</v>
       </c>
@@ -2493,11 +2497,11 @@
     </row>
     <row r="21" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="17"/>
-      <c r="B21" s="107"/>
+      <c r="B21" s="112"/>
       <c r="C21" s="2"/>
       <c r="D21" s="11"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="103"/>
+      <c r="E21" s="99"/>
+      <c r="F21" s="132"/>
       <c r="G21" s="14" t="s">
         <v>24</v>
       </c>
@@ -2520,10 +2524,10 @@
     </row>
     <row r="22" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="17"/>
-      <c r="B22" s="107"/>
+      <c r="B22" s="112"/>
       <c r="C22" s="2"/>
       <c r="D22" s="11"/>
-      <c r="E22" s="104"/>
+      <c r="E22" s="116"/>
       <c r="F22" s="60"/>
       <c r="G22" s="14" t="s">
         <v>42</v>
@@ -2551,7 +2555,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23" s="17"/>
-      <c r="B23" s="107"/>
+      <c r="B23" s="112"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -2574,13 +2578,13 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24" s="17"/>
-      <c r="B24" s="107"/>
+      <c r="B24" s="112"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="94" t="s">
+      <c r="E24" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="98" t="s">
+      <c r="F24" s="106" t="s">
         <v>45</v>
       </c>
       <c r="G24" s="39" t="s">
@@ -2605,11 +2609,11 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25" s="17"/>
-      <c r="B25" s="107"/>
+      <c r="B25" s="112"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="99"/>
+      <c r="E25" s="99"/>
+      <c r="F25" s="107"/>
       <c r="G25" s="6" t="s">
         <v>26</v>
       </c>
@@ -2632,11 +2636,11 @@
     </row>
     <row r="26" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="17"/>
-      <c r="B26" s="107"/>
+      <c r="B26" s="112"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="100"/>
+      <c r="E26" s="99"/>
+      <c r="F26" s="108"/>
       <c r="G26" s="14" t="s">
         <v>24</v>
       </c>
@@ -2659,10 +2663,10 @@
     </row>
     <row r="27" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
-      <c r="B27" s="107"/>
+      <c r="B27" s="112"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="95"/>
+      <c r="E27" s="103"/>
       <c r="F27" s="33"/>
       <c r="G27" s="8" t="s">
         <v>42</v>
@@ -2690,7 +2694,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A28" s="17"/>
-      <c r="B28" s="107"/>
+      <c r="B28" s="112"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="9"/>
@@ -2713,7 +2717,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A29" s="17"/>
-      <c r="B29" s="107"/>
+      <c r="B29" s="112"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
@@ -2736,17 +2740,17 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30" s="17"/>
-      <c r="B30" s="107"/>
+      <c r="B30" s="112"/>
       <c r="C30" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="94" t="s">
+      <c r="E30" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="91" t="s">
+      <c r="F30" s="100" t="s">
         <v>5</v>
       </c>
       <c r="G30" s="39" t="s">
@@ -2771,11 +2775,11 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31" s="17"/>
-      <c r="B31" s="107"/>
+      <c r="B31" s="112"/>
       <c r="C31" s="2"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="92"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="101"/>
       <c r="G31" s="6" t="s">
         <v>26</v>
       </c>
@@ -2798,11 +2802,11 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32" s="17"/>
-      <c r="B32" s="107"/>
+      <c r="B32" s="112"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="93"/>
+      <c r="E32" s="99"/>
+      <c r="F32" s="102"/>
       <c r="G32" s="14" t="s">
         <v>24</v>
       </c>
@@ -2825,7 +2829,7 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A33" s="17"/>
-      <c r="B33" s="107"/>
+      <c r="B33" s="112"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="35"/>
@@ -2848,13 +2852,13 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A34" s="17"/>
-      <c r="B34" s="107"/>
+      <c r="B34" s="112"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="94" t="s">
+      <c r="E34" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="91" t="s">
+      <c r="F34" s="100" t="s">
         <v>5</v>
       </c>
       <c r="G34" s="39" t="s">
@@ -2879,11 +2883,11 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A35" s="17"/>
-      <c r="B35" s="107"/>
+      <c r="B35" s="112"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="92"/>
+      <c r="E35" s="99"/>
+      <c r="F35" s="101"/>
       <c r="G35" s="6" t="s">
         <v>26</v>
       </c>
@@ -2906,11 +2910,11 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A36" s="17"/>
-      <c r="B36" s="107"/>
+      <c r="B36" s="112"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="93"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="102"/>
       <c r="G36" s="14" t="s">
         <v>24</v>
       </c>
@@ -2933,18 +2937,18 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A37" s="17"/>
-      <c r="B37" s="107"/>
+      <c r="B37" s="112"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="89"/>
+      <c r="E37" s="99"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="82" t="s">
+      <c r="G37" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H37" s="83">
+      <c r="H37" s="30">
         <v>1</v>
       </c>
-      <c r="I37" s="83" t="s">
+      <c r="I37" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J37" s="30"/>
@@ -2964,18 +2968,18 @@
     </row>
     <row r="38" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A38" s="17"/>
-      <c r="B38" s="107"/>
+      <c r="B38" s="112"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="89"/>
+      <c r="E38" s="99"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="82" t="s">
+      <c r="G38" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H38" s="83">
+      <c r="H38" s="30">
         <v>1</v>
       </c>
-      <c r="I38" s="83"/>
+      <c r="I38" s="30"/>
       <c r="J38" s="30"/>
       <c r="K38" s="31"/>
       <c r="L38" s="38"/>
@@ -2991,18 +2995,18 @@
     </row>
     <row r="39" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="17"/>
-      <c r="B39" s="107"/>
+      <c r="B39" s="112"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="89"/>
+      <c r="E39" s="99"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="82" t="s">
+      <c r="G39" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H39" s="83">
+      <c r="H39" s="30">
         <v>2</v>
       </c>
-      <c r="I39" s="83" t="s">
+      <c r="I39" s="30" t="s">
         <v>76</v>
       </c>
       <c r="J39" s="30"/>
@@ -3020,18 +3024,18 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A40" s="17"/>
-      <c r="B40" s="107"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="89"/>
+      <c r="E40" s="99"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="82" t="s">
+      <c r="G40" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H40" s="84">
+      <c r="H40" s="136">
         <v>16</v>
       </c>
-      <c r="I40" s="84" t="s">
+      <c r="I40" s="136" t="s">
         <v>53</v>
       </c>
       <c r="J40" s="30"/>
@@ -3049,18 +3053,18 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A41" s="17"/>
-      <c r="B41" s="107"/>
+      <c r="B41" s="112"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="89"/>
+      <c r="E41" s="99"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="82" t="s">
+      <c r="G41" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H41" s="83">
+      <c r="H41" s="30">
         <v>4</v>
       </c>
-      <c r="I41" s="83" t="s">
+      <c r="I41" s="30" t="s">
         <v>62</v>
       </c>
       <c r="J41" s="30"/>
@@ -3078,18 +3082,18 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A42" s="17"/>
-      <c r="B42" s="107"/>
+      <c r="B42" s="112"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="89"/>
+      <c r="E42" s="99"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="82" t="s">
+      <c r="G42" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H42" s="83">
+      <c r="H42" s="30">
         <v>1</v>
       </c>
-      <c r="I42" s="83" t="s">
+      <c r="I42" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J42" s="30"/>
@@ -3107,18 +3111,18 @@
     </row>
     <row r="43" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="17"/>
-      <c r="B43" s="107"/>
+      <c r="B43" s="112"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="89"/>
+      <c r="E43" s="99"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="82" t="s">
+      <c r="G43" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H43" s="83">
+      <c r="H43" s="30">
         <v>1</v>
       </c>
-      <c r="I43" s="83" t="s">
+      <c r="I43" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J43" s="30"/>
@@ -3136,18 +3140,18 @@
     </row>
     <row r="44" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
-      <c r="B44" s="107"/>
+      <c r="B44" s="112"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
-      <c r="E44" s="95"/>
+      <c r="E44" s="103"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="85" t="s">
+      <c r="G44" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="H44" s="86">
+      <c r="H44" s="62">
         <v>2</v>
       </c>
-      <c r="I44" s="86"/>
+      <c r="I44" s="62"/>
       <c r="J44" s="37"/>
       <c r="K44" s="44"/>
       <c r="L44" s="45"/>
@@ -3163,7 +3167,7 @@
     </row>
     <row r="45" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A45" s="17"/>
-      <c r="B45" s="107"/>
+      <c r="B45" s="112"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="9"/>
@@ -3186,7 +3190,7 @@
     </row>
     <row r="46" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A46" s="17"/>
-      <c r="B46" s="107"/>
+      <c r="B46" s="112"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="9"/>
@@ -3209,17 +3213,17 @@
     </row>
     <row r="47" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A47" s="17"/>
-      <c r="B47" s="107"/>
+      <c r="B47" s="112"/>
       <c r="C47" s="34" t="s">
         <v>71</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E47" s="94" t="s">
+      <c r="E47" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="91" t="s">
+      <c r="F47" s="100" t="s">
         <v>5</v>
       </c>
       <c r="G47" s="39" t="s">
@@ -3244,11 +3248,11 @@
     </row>
     <row r="48" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A48" s="17"/>
-      <c r="B48" s="107"/>
+      <c r="B48" s="112"/>
       <c r="C48" s="2"/>
       <c r="D48" s="11"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="92"/>
+      <c r="E48" s="99"/>
+      <c r="F48" s="101"/>
       <c r="G48" s="6" t="s">
         <v>26</v>
       </c>
@@ -3271,11 +3275,11 @@
     </row>
     <row r="49" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A49" s="17"/>
-      <c r="B49" s="107"/>
+      <c r="B49" s="112"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="93"/>
+      <c r="E49" s="99"/>
+      <c r="F49" s="102"/>
       <c r="G49" s="14" t="s">
         <v>24</v>
       </c>
@@ -3298,7 +3302,7 @@
     </row>
     <row r="50" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A50" s="17"/>
-      <c r="B50" s="107"/>
+      <c r="B50" s="112"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="35"/>
@@ -3321,13 +3325,13 @@
     </row>
     <row r="51" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A51" s="17"/>
-      <c r="B51" s="107"/>
+      <c r="B51" s="112"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="94" t="s">
+      <c r="E51" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="F51" s="91" t="s">
+      <c r="F51" s="100" t="s">
         <v>5</v>
       </c>
       <c r="G51" s="39" t="s">
@@ -3352,11 +3356,11 @@
     </row>
     <row r="52" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A52" s="17"/>
-      <c r="B52" s="107"/>
+      <c r="B52" s="112"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="89"/>
-      <c r="F52" s="92"/>
+      <c r="E52" s="99"/>
+      <c r="F52" s="101"/>
       <c r="G52" s="6" t="s">
         <v>26</v>
       </c>
@@ -3379,11 +3383,11 @@
     </row>
     <row r="53" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A53" s="17"/>
-      <c r="B53" s="107"/>
+      <c r="B53" s="112"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="89"/>
-      <c r="F53" s="93"/>
+      <c r="E53" s="99"/>
+      <c r="F53" s="102"/>
       <c r="G53" s="14" t="s">
         <v>24</v>
       </c>
@@ -3406,10 +3410,10 @@
     </row>
     <row r="54" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A54" s="17"/>
-      <c r="B54" s="107"/>
+      <c r="B54" s="112"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="89"/>
+      <c r="E54" s="99"/>
       <c r="F54" s="2"/>
       <c r="G54" s="6" t="s">
         <v>72</v>
@@ -3435,10 +3439,10 @@
     </row>
     <row r="55" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A55" s="17"/>
-      <c r="B55" s="107"/>
+      <c r="B55" s="112"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="89"/>
+      <c r="E55" s="99"/>
       <c r="F55" s="2"/>
       <c r="G55" s="6" t="s">
         <v>73</v>
@@ -3464,10 +3468,10 @@
     </row>
     <row r="56" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A56" s="17"/>
-      <c r="B56" s="107"/>
+      <c r="B56" s="112"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="89"/>
+      <c r="E56" s="99"/>
       <c r="F56" s="2"/>
       <c r="G56" s="6" t="s">
         <v>74</v>
@@ -3493,10 +3497,10 @@
     </row>
     <row r="57" spans="1:21" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
-      <c r="B57" s="107"/>
+      <c r="B57" s="112"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
-      <c r="E57" s="95"/>
+      <c r="E57" s="103"/>
       <c r="F57" s="7"/>
       <c r="G57" s="61" t="s">
         <v>75</v>
@@ -3522,7 +3526,7 @@
     </row>
     <row r="58" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A58" s="17"/>
-      <c r="B58" s="107"/>
+      <c r="B58" s="112"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="9"/>
@@ -3532,7 +3536,7 @@
       <c r="I58" s="30"/>
       <c r="J58" s="30"/>
       <c r="K58" s="30"/>
-      <c r="L58" s="135"/>
+      <c r="L58" s="94"/>
       <c r="M58" s="16"/>
       <c r="N58" s="16"/>
       <c r="O58" s="16"/>
@@ -3545,7 +3549,7 @@
     </row>
     <row r="59" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A59" s="17"/>
-      <c r="B59" s="107"/>
+      <c r="B59" s="112"/>
       <c r="C59" s="17"/>
       <c r="D59" s="17"/>
       <c r="E59" s="2"/>
@@ -3568,17 +3572,17 @@
     </row>
     <row r="60" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A60" s="17"/>
-      <c r="B60" s="107"/>
+      <c r="B60" s="112"/>
       <c r="C60" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="E60" s="94" t="s">
+        <v>138</v>
+      </c>
+      <c r="E60" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="F60" s="91" t="s">
+      <c r="F60" s="100" t="s">
         <v>5</v>
       </c>
       <c r="G60" s="39" t="s">
@@ -3603,11 +3607,11 @@
     </row>
     <row r="61" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A61" s="17"/>
-      <c r="B61" s="107"/>
+      <c r="B61" s="112"/>
       <c r="C61" s="2"/>
       <c r="D61" s="11"/>
-      <c r="E61" s="89"/>
-      <c r="F61" s="92"/>
+      <c r="E61" s="99"/>
+      <c r="F61" s="101"/>
       <c r="G61" s="6" t="s">
         <v>26</v>
       </c>
@@ -3630,11 +3634,11 @@
     </row>
     <row r="62" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A62" s="17"/>
-      <c r="B62" s="107"/>
+      <c r="B62" s="112"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
-      <c r="E62" s="89"/>
-      <c r="F62" s="93"/>
+      <c r="E62" s="99"/>
+      <c r="F62" s="102"/>
       <c r="G62" s="14" t="s">
         <v>24</v>
       </c>
@@ -3657,7 +3661,7 @@
     </row>
     <row r="63" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A63" s="17"/>
-      <c r="B63" s="107"/>
+      <c r="B63" s="112"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="35"/>
@@ -3680,13 +3684,13 @@
     </row>
     <row r="64" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A64" s="17"/>
-      <c r="B64" s="107"/>
+      <c r="B64" s="112"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="94" t="s">
+      <c r="E64" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="F64" s="91" t="s">
+      <c r="F64" s="100" t="s">
         <v>5</v>
       </c>
       <c r="G64" s="39" t="s">
@@ -3711,11 +3715,11 @@
     </row>
     <row r="65" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A65" s="17"/>
-      <c r="B65" s="107"/>
+      <c r="B65" s="112"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="89"/>
-      <c r="F65" s="92"/>
+      <c r="E65" s="99"/>
+      <c r="F65" s="101"/>
       <c r="G65" s="6" t="s">
         <v>26</v>
       </c>
@@ -3738,11 +3742,11 @@
     </row>
     <row r="66" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A66" s="17"/>
-      <c r="B66" s="107"/>
+      <c r="B66" s="112"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="89"/>
-      <c r="F66" s="93"/>
+      <c r="E66" s="99"/>
+      <c r="F66" s="102"/>
       <c r="G66" s="14" t="s">
         <v>24</v>
       </c>
@@ -3765,18 +3769,18 @@
     </row>
     <row r="67" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A67" s="17"/>
-      <c r="B67" s="107"/>
+      <c r="B67" s="112"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="89"/>
+      <c r="E67" s="99"/>
       <c r="F67" s="2"/>
-      <c r="G67" s="82" t="s">
+      <c r="G67" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H67" s="83">
+      <c r="H67" s="30">
         <v>1</v>
       </c>
-      <c r="I67" s="83" t="s">
+      <c r="I67" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J67" s="30"/>
@@ -3794,18 +3798,18 @@
     </row>
     <row r="68" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A68" s="17"/>
-      <c r="B68" s="107"/>
+      <c r="B68" s="112"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
-      <c r="E68" s="89"/>
+      <c r="E68" s="99"/>
       <c r="F68" s="2"/>
-      <c r="G68" s="82" t="s">
+      <c r="G68" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H68" s="83">
+      <c r="H68" s="30">
         <v>3</v>
       </c>
-      <c r="I68" s="83" t="s">
+      <c r="I68" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J68" s="30"/>
@@ -3823,20 +3827,20 @@
     </row>
     <row r="69" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A69" s="17"/>
-      <c r="B69" s="107"/>
+      <c r="B69" s="112"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
-      <c r="E69" s="89"/>
-      <c r="F69" s="120" t="s">
-        <v>105</v>
-      </c>
-      <c r="G69" s="82" t="s">
+      <c r="E69" s="99"/>
+      <c r="F69" s="104" t="s">
+        <v>104</v>
+      </c>
+      <c r="G69" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H69" s="83">
+      <c r="H69" s="30">
         <v>8</v>
       </c>
-      <c r="I69" s="83" t="s">
+      <c r="I69" s="30" t="s">
         <v>63</v>
       </c>
       <c r="J69" s="30"/>
@@ -3854,19 +3858,19 @@
     </row>
     <row r="70" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A70" s="17"/>
-      <c r="B70" s="107"/>
+      <c r="B70" s="112"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="89"/>
-      <c r="F70" s="120"/>
-      <c r="G70" s="82" t="s">
-        <v>118</v>
-      </c>
-      <c r="H70" s="83">
+      <c r="E70" s="99"/>
+      <c r="F70" s="104"/>
+      <c r="G70" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H70" s="30">
         <v>1</v>
       </c>
-      <c r="I70" s="83" t="s">
-        <v>113</v>
+      <c r="I70" s="30" t="s">
+        <v>111</v>
       </c>
       <c r="J70" s="30"/>
       <c r="K70" s="31"/>
@@ -3883,19 +3887,19 @@
     </row>
     <row r="71" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A71" s="17"/>
-      <c r="B71" s="107"/>
+      <c r="B71" s="112"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
-      <c r="E71" s="89"/>
-      <c r="F71" s="120"/>
-      <c r="G71" s="82" t="s">
+      <c r="E71" s="99"/>
+      <c r="F71" s="104"/>
+      <c r="G71" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H71" s="83">
+      <c r="H71" s="30">
         <v>1</v>
       </c>
-      <c r="I71" s="83" t="s">
-        <v>113</v>
+      <c r="I71" s="30" t="s">
+        <v>111</v>
       </c>
       <c r="J71" s="30"/>
       <c r="K71" s="31"/>
@@ -3912,18 +3916,18 @@
     </row>
     <row r="72" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A72" s="17"/>
-      <c r="B72" s="107"/>
+      <c r="B72" s="112"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
-      <c r="E72" s="89"/>
-      <c r="F72" s="120"/>
-      <c r="G72" s="82" t="s">
+      <c r="E72" s="99"/>
+      <c r="F72" s="104"/>
+      <c r="G72" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H72" s="83">
+      <c r="H72" s="30">
         <v>2</v>
       </c>
-      <c r="I72" s="83"/>
+      <c r="I72" s="30"/>
       <c r="J72" s="30"/>
       <c r="K72" s="31"/>
       <c r="L72" s="38"/>
@@ -3939,19 +3943,19 @@
     </row>
     <row r="73" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A73" s="17"/>
-      <c r="B73" s="107"/>
+      <c r="B73" s="112"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
-      <c r="E73" s="89"/>
-      <c r="F73" s="120"/>
-      <c r="G73" s="82" t="s">
-        <v>107</v>
-      </c>
-      <c r="H73" s="83">
+      <c r="E73" s="99"/>
+      <c r="F73" s="104"/>
+      <c r="G73" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H73" s="30">
         <v>16</v>
       </c>
-      <c r="I73" s="83" t="s">
-        <v>104</v>
+      <c r="I73" s="30" t="s">
+        <v>103</v>
       </c>
       <c r="J73" s="30"/>
       <c r="K73" s="31"/>
@@ -3968,19 +3972,19 @@
     </row>
     <row r="74" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A74" s="17"/>
-      <c r="B74" s="107"/>
+      <c r="B74" s="112"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
-      <c r="E74" s="89"/>
-      <c r="F74" s="120"/>
-      <c r="G74" s="82" t="s">
-        <v>112</v>
-      </c>
-      <c r="H74" s="83">
+      <c r="E74" s="99"/>
+      <c r="F74" s="104"/>
+      <c r="G74" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H74" s="30">
         <v>32</v>
       </c>
-      <c r="I74" s="83" t="s">
-        <v>104</v>
+      <c r="I74" s="30" t="s">
+        <v>103</v>
       </c>
       <c r="J74" s="30"/>
       <c r="K74" s="31"/>
@@ -3997,16 +4001,16 @@
     </row>
     <row r="75" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A75" s="17"/>
-      <c r="B75" s="107"/>
+      <c r="B75" s="112"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
-      <c r="E75" s="89"/>
-      <c r="F75" s="119" t="s">
-        <v>106</v>
-      </c>
-      <c r="G75" s="82"/>
-      <c r="H75" s="83"/>
-      <c r="I75" s="83"/>
+      <c r="E75" s="99"/>
+      <c r="F75" s="88" t="s">
+        <v>105</v>
+      </c>
+      <c r="G75" s="6"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="30"/>
       <c r="J75" s="30"/>
       <c r="K75" s="31"/>
       <c r="L75" s="38"/>
@@ -4022,20 +4026,20 @@
     </row>
     <row r="76" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A76" s="17"/>
-      <c r="B76" s="107"/>
+      <c r="B76" s="112"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="89"/>
-      <c r="F76" s="120" t="s">
-        <v>108</v>
-      </c>
-      <c r="G76" s="82" t="s">
+      <c r="E76" s="99"/>
+      <c r="F76" s="104" t="s">
+        <v>107</v>
+      </c>
+      <c r="G76" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H76" s="83">
+      <c r="H76" s="30">
         <v>8</v>
       </c>
-      <c r="I76" s="83" t="s">
+      <c r="I76" s="30" t="s">
         <v>63</v>
       </c>
       <c r="J76" s="30"/>
@@ -4053,19 +4057,19 @@
     </row>
     <row r="77" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A77" s="17"/>
-      <c r="B77" s="107"/>
+      <c r="B77" s="112"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
-      <c r="E77" s="89"/>
-      <c r="F77" s="120"/>
-      <c r="G77" s="82" t="s">
-        <v>118</v>
-      </c>
-      <c r="H77" s="83">
+      <c r="E77" s="99"/>
+      <c r="F77" s="104"/>
+      <c r="G77" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H77" s="30">
         <v>1</v>
       </c>
-      <c r="I77" s="83" t="s">
-        <v>113</v>
+      <c r="I77" s="30" t="s">
+        <v>111</v>
       </c>
       <c r="J77" s="30"/>
       <c r="K77" s="31"/>
@@ -4082,19 +4086,19 @@
     </row>
     <row r="78" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A78" s="17"/>
-      <c r="B78" s="107"/>
+      <c r="B78" s="112"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="89"/>
-      <c r="F78" s="120"/>
-      <c r="G78" s="82" t="s">
+      <c r="E78" s="99"/>
+      <c r="F78" s="104"/>
+      <c r="G78" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H78" s="83">
+      <c r="H78" s="30">
         <v>1</v>
       </c>
-      <c r="I78" s="83" t="s">
-        <v>113</v>
+      <c r="I78" s="30" t="s">
+        <v>111</v>
       </c>
       <c r="J78" s="30"/>
       <c r="K78" s="31"/>
@@ -4111,18 +4115,18 @@
     </row>
     <row r="79" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A79" s="17"/>
-      <c r="B79" s="107"/>
+      <c r="B79" s="112"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
-      <c r="E79" s="89"/>
-      <c r="F79" s="120"/>
-      <c r="G79" s="82" t="s">
+      <c r="E79" s="99"/>
+      <c r="F79" s="104"/>
+      <c r="G79" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H79" s="83">
+      <c r="H79" s="30">
         <v>2</v>
       </c>
-      <c r="I79" s="83"/>
+      <c r="I79" s="30"/>
       <c r="J79" s="30"/>
       <c r="K79" s="31"/>
       <c r="L79" s="38"/>
@@ -4138,19 +4142,19 @@
     </row>
     <row r="80" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A80" s="17"/>
-      <c r="B80" s="107"/>
+      <c r="B80" s="112"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
-      <c r="E80" s="89"/>
-      <c r="F80" s="120"/>
-      <c r="G80" s="82" t="s">
-        <v>107</v>
-      </c>
-      <c r="H80" s="83">
+      <c r="E80" s="99"/>
+      <c r="F80" s="104"/>
+      <c r="G80" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H80" s="30">
         <v>16</v>
       </c>
-      <c r="I80" s="83" t="s">
-        <v>104</v>
+      <c r="I80" s="30" t="s">
+        <v>103</v>
       </c>
       <c r="J80" s="30"/>
       <c r="K80" s="31"/>
@@ -4167,23 +4171,23 @@
     </row>
     <row r="81" spans="1:21" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A81" s="17"/>
-      <c r="B81" s="107"/>
+      <c r="B81" s="112"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
-      <c r="E81" s="95"/>
-      <c r="F81" s="121"/>
-      <c r="G81" s="85" t="s">
-        <v>114</v>
-      </c>
-      <c r="H81" s="86">
+      <c r="E81" s="103"/>
+      <c r="F81" s="105"/>
+      <c r="G81" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="H81" s="62">
         <v>32</v>
       </c>
-      <c r="I81" s="86" t="s">
+      <c r="I81" s="62" t="s">
         <v>53</v>
       </c>
       <c r="J81" s="37"/>
       <c r="K81" s="44"/>
-      <c r="L81" s="132"/>
+      <c r="L81" s="91"/>
       <c r="M81" s="16"/>
       <c r="N81" s="16"/>
       <c r="O81" s="16"/>
@@ -4196,7 +4200,7 @@
     </row>
     <row r="82" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A82" s="17"/>
-      <c r="B82" s="107"/>
+      <c r="B82" s="112"/>
       <c r="C82" s="17"/>
       <c r="D82" s="17"/>
       <c r="E82" s="2"/>
@@ -4219,7 +4223,7 @@
     </row>
     <row r="83" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A83" s="17"/>
-      <c r="B83" s="107"/>
+      <c r="B83" s="112"/>
       <c r="C83" s="17"/>
       <c r="D83" s="17"/>
       <c r="E83" s="2"/>
@@ -4242,17 +4246,17 @@
     </row>
     <row r="84" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A84" s="17"/>
-      <c r="B84" s="107"/>
+      <c r="B84" s="112"/>
       <c r="C84" s="34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="E84" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="E84" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="F84" s="91" t="s">
+      <c r="F84" s="100" t="s">
         <v>5</v>
       </c>
       <c r="G84" s="39" t="s">
@@ -4277,11 +4281,11 @@
     </row>
     <row r="85" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A85" s="17"/>
-      <c r="B85" s="107"/>
+      <c r="B85" s="112"/>
       <c r="C85" s="2"/>
       <c r="D85" s="11"/>
-      <c r="E85" s="89"/>
-      <c r="F85" s="92"/>
+      <c r="E85" s="99"/>
+      <c r="F85" s="101"/>
       <c r="G85" s="6" t="s">
         <v>26</v>
       </c>
@@ -4304,11 +4308,11 @@
     </row>
     <row r="86" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A86" s="17"/>
-      <c r="B86" s="107"/>
+      <c r="B86" s="112"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
-      <c r="E86" s="89"/>
-      <c r="F86" s="93"/>
+      <c r="E86" s="99"/>
+      <c r="F86" s="102"/>
       <c r="G86" s="14" t="s">
         <v>24</v>
       </c>
@@ -4331,7 +4335,7 @@
     </row>
     <row r="87" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A87" s="17"/>
-      <c r="B87" s="107"/>
+      <c r="B87" s="112"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="35"/>
@@ -4354,13 +4358,13 @@
     </row>
     <row r="88" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A88" s="17"/>
-      <c r="B88" s="107"/>
+      <c r="B88" s="112"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
-      <c r="E88" s="94" t="s">
+      <c r="E88" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="F88" s="91" t="s">
+      <c r="F88" s="100" t="s">
         <v>5</v>
       </c>
       <c r="G88" s="39" t="s">
@@ -4385,11 +4389,11 @@
     </row>
     <row r="89" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A89" s="17"/>
-      <c r="B89" s="107"/>
+      <c r="B89" s="112"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="89"/>
-      <c r="F89" s="92"/>
+      <c r="E89" s="99"/>
+      <c r="F89" s="101"/>
       <c r="G89" s="6" t="s">
         <v>26</v>
       </c>
@@ -4412,11 +4416,11 @@
     </row>
     <row r="90" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A90" s="17"/>
-      <c r="B90" s="107"/>
+      <c r="B90" s="112"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
-      <c r="E90" s="89"/>
-      <c r="F90" s="93"/>
+      <c r="E90" s="99"/>
+      <c r="F90" s="102"/>
       <c r="G90" s="14" t="s">
         <v>24</v>
       </c>
@@ -4439,18 +4443,18 @@
     </row>
     <row r="91" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A91" s="17"/>
-      <c r="B91" s="107"/>
+      <c r="B91" s="112"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
-      <c r="E91" s="89"/>
+      <c r="E91" s="99"/>
       <c r="F91" s="2"/>
-      <c r="G91" s="82" t="s">
+      <c r="G91" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H91" s="83">
+      <c r="H91" s="30">
         <v>1</v>
       </c>
-      <c r="I91" s="83" t="s">
+      <c r="I91" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J91" s="30"/>
@@ -4468,18 +4472,18 @@
     </row>
     <row r="92" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A92" s="17"/>
-      <c r="B92" s="107"/>
+      <c r="B92" s="112"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
-      <c r="E92" s="89"/>
+      <c r="E92" s="99"/>
       <c r="F92" s="2"/>
-      <c r="G92" s="82" t="s">
+      <c r="G92" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H92" s="83">
+      <c r="H92" s="30">
         <v>3</v>
       </c>
-      <c r="I92" s="83" t="s">
+      <c r="I92" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J92" s="30"/>
@@ -4497,20 +4501,20 @@
     </row>
     <row r="93" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A93" s="17"/>
-      <c r="B93" s="107"/>
+      <c r="B93" s="112"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
-      <c r="E93" s="89"/>
-      <c r="F93" s="120" t="s">
-        <v>105</v>
-      </c>
-      <c r="G93" s="82" t="s">
+      <c r="E93" s="99"/>
+      <c r="F93" s="104" t="s">
+        <v>104</v>
+      </c>
+      <c r="G93" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H93" s="83">
+      <c r="H93" s="30">
         <v>8</v>
       </c>
-      <c r="I93" s="83" t="s">
+      <c r="I93" s="30" t="s">
         <v>63</v>
       </c>
       <c r="J93" s="30"/>
@@ -4528,19 +4532,19 @@
     </row>
     <row r="94" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A94" s="17"/>
-      <c r="B94" s="107"/>
+      <c r="B94" s="112"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
-      <c r="E94" s="89"/>
-      <c r="F94" s="120"/>
-      <c r="G94" s="82" t="s">
-        <v>126</v>
-      </c>
-      <c r="H94" s="83">
+      <c r="E94" s="99"/>
+      <c r="F94" s="104"/>
+      <c r="G94" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H94" s="30">
         <v>16</v>
       </c>
-      <c r="I94" s="83" t="s">
-        <v>104</v>
+      <c r="I94" s="30" t="s">
+        <v>103</v>
       </c>
       <c r="J94" s="30"/>
       <c r="K94" s="31"/>
@@ -4559,16 +4563,16 @@
     </row>
     <row r="95" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A95" s="17"/>
-      <c r="B95" s="107"/>
+      <c r="B95" s="112"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="89"/>
+      <c r="E95" s="99"/>
       <c r="F95" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G95" s="82"/>
-      <c r="H95" s="83"/>
-      <c r="I95" s="83"/>
+        <v>105</v>
+      </c>
+      <c r="G95" s="6"/>
+      <c r="H95" s="30"/>
+      <c r="I95" s="30"/>
       <c r="J95" s="30"/>
       <c r="K95" s="31"/>
       <c r="L95" s="38"/>
@@ -4584,20 +4588,20 @@
     </row>
     <row r="96" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A96" s="17"/>
-      <c r="B96" s="107"/>
+      <c r="B96" s="112"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
-      <c r="E96" s="89"/>
-      <c r="F96" s="120" t="s">
+      <c r="E96" s="99"/>
+      <c r="F96" s="104" t="s">
+        <v>107</v>
+      </c>
+      <c r="G96" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="G96" s="82" t="s">
-        <v>109</v>
-      </c>
-      <c r="H96" s="83">
+      <c r="H96" s="30">
         <v>8</v>
       </c>
-      <c r="I96" s="83" t="s">
+      <c r="I96" s="30" t="s">
         <v>53</v>
       </c>
       <c r="J96" s="30"/>
@@ -4615,18 +4619,18 @@
     </row>
     <row r="97" spans="1:21" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A97" s="17"/>
-      <c r="B97" s="107"/>
+      <c r="B97" s="112"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
-      <c r="E97" s="95"/>
-      <c r="F97" s="121"/>
-      <c r="G97" s="85" t="s">
-        <v>126</v>
-      </c>
-      <c r="H97" s="86">
+      <c r="E97" s="103"/>
+      <c r="F97" s="105"/>
+      <c r="G97" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="H97" s="62">
         <v>16</v>
       </c>
-      <c r="I97" s="86" t="s">
+      <c r="I97" s="62" t="s">
         <v>53</v>
       </c>
       <c r="J97" s="37"/>
@@ -4646,7 +4650,7 @@
     </row>
     <row r="98" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A98" s="17"/>
-      <c r="B98" s="107"/>
+      <c r="B98" s="112"/>
       <c r="C98" s="17"/>
       <c r="D98" s="17"/>
       <c r="E98" s="2"/>
@@ -4669,7 +4673,7 @@
     </row>
     <row r="99" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A99" s="17"/>
-      <c r="B99" s="107"/>
+      <c r="B99" s="112"/>
       <c r="C99" s="17"/>
       <c r="D99" s="17"/>
       <c r="E99" s="2"/>
@@ -4692,17 +4696,17 @@
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A100" s="17"/>
-      <c r="B100" s="107"/>
+      <c r="B100" s="112"/>
       <c r="C100" s="70" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D100" s="71" t="s">
-        <v>117</v>
-      </c>
-      <c r="E100" s="108" t="s">
+        <v>115</v>
+      </c>
+      <c r="E100" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="F100" s="113" t="s">
+      <c r="F100" s="121" t="s">
         <v>5</v>
       </c>
       <c r="G100" s="63" t="s">
@@ -4727,11 +4731,11 @@
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A101" s="17"/>
-      <c r="B101" s="107"/>
+      <c r="B101" s="112"/>
       <c r="C101" s="13"/>
       <c r="D101" s="11"/>
-      <c r="E101" s="109"/>
-      <c r="F101" s="114"/>
+      <c r="E101" s="114"/>
+      <c r="F101" s="122"/>
       <c r="G101" s="6" t="s">
         <v>26</v>
       </c>
@@ -4754,11 +4758,11 @@
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A102" s="17"/>
-      <c r="B102" s="107"/>
+      <c r="B102" s="112"/>
       <c r="C102" s="13"/>
       <c r="D102" s="2"/>
-      <c r="E102" s="110"/>
-      <c r="F102" s="122"/>
+      <c r="E102" s="115"/>
+      <c r="F102" s="128"/>
       <c r="G102" s="67" t="s">
         <v>24</v>
       </c>
@@ -4781,7 +4785,7 @@
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A103" s="17"/>
-      <c r="B103" s="107"/>
+      <c r="B103" s="112"/>
       <c r="C103" s="13"/>
       <c r="D103" s="2"/>
       <c r="E103" s="75"/>
@@ -4804,13 +4808,13 @@
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A104" s="17"/>
-      <c r="B104" s="107"/>
+      <c r="B104" s="112"/>
       <c r="C104" s="13"/>
       <c r="D104" s="2"/>
-      <c r="E104" s="94" t="s">
+      <c r="E104" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="F104" s="91" t="s">
+      <c r="F104" s="100" t="s">
         <v>5</v>
       </c>
       <c r="G104" s="39" t="s">
@@ -4835,11 +4839,11 @@
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A105" s="17"/>
-      <c r="B105" s="107"/>
+      <c r="B105" s="112"/>
       <c r="C105" s="13"/>
       <c r="D105" s="2"/>
-      <c r="E105" s="89"/>
-      <c r="F105" s="92"/>
+      <c r="E105" s="99"/>
+      <c r="F105" s="101"/>
       <c r="G105" s="6" t="s">
         <v>26</v>
       </c>
@@ -4862,11 +4866,11 @@
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A106" s="17"/>
-      <c r="B106" s="107"/>
+      <c r="B106" s="112"/>
       <c r="C106" s="13"/>
       <c r="D106" s="2"/>
-      <c r="E106" s="89"/>
-      <c r="F106" s="93"/>
+      <c r="E106" s="99"/>
+      <c r="F106" s="102"/>
       <c r="G106" s="67" t="s">
         <v>24</v>
       </c>
@@ -4889,18 +4893,18 @@
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A107" s="17"/>
-      <c r="B107" s="107"/>
+      <c r="B107" s="112"/>
       <c r="C107" s="13"/>
       <c r="D107" s="2"/>
-      <c r="E107" s="89"/>
-      <c r="F107" s="111"/>
-      <c r="G107" s="82" t="s">
+      <c r="E107" s="99"/>
+      <c r="F107" s="117"/>
+      <c r="G107" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H107" s="83">
+      <c r="H107" s="30">
         <v>1</v>
       </c>
-      <c r="I107" s="83" t="s">
+      <c r="I107" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J107" s="30"/>
@@ -4918,18 +4922,18 @@
     </row>
     <row r="108" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A108" s="17"/>
-      <c r="B108" s="107"/>
+      <c r="B108" s="112"/>
       <c r="C108" s="13"/>
       <c r="D108" s="2"/>
-      <c r="E108" s="89"/>
-      <c r="F108" s="112"/>
-      <c r="G108" s="82" t="s">
+      <c r="E108" s="99"/>
+      <c r="F108" s="118"/>
+      <c r="G108" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H108" s="83">
+      <c r="H108" s="30">
         <v>3</v>
       </c>
-      <c r="I108" s="83" t="s">
+      <c r="I108" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J108" s="30"/>
@@ -4947,20 +4951,20 @@
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A109" s="17"/>
-      <c r="B109" s="107"/>
+      <c r="B109" s="112"/>
       <c r="C109" s="13"/>
       <c r="D109" s="2"/>
-      <c r="E109" s="89"/>
-      <c r="F109" s="96" t="s">
+      <c r="E109" s="99"/>
+      <c r="F109" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="G109" s="82" t="s">
+      <c r="G109" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H109" s="83">
+      <c r="H109" s="30">
         <v>8</v>
       </c>
-      <c r="I109" s="83" t="s">
+      <c r="I109" s="30" t="s">
         <v>63</v>
       </c>
       <c r="J109" s="30"/>
@@ -4978,18 +4982,18 @@
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A110" s="17"/>
-      <c r="B110" s="107"/>
+      <c r="B110" s="112"/>
       <c r="C110" s="13"/>
       <c r="D110" s="2"/>
-      <c r="E110" s="89"/>
-      <c r="F110" s="96"/>
-      <c r="G110" s="82" t="s">
+      <c r="E110" s="99"/>
+      <c r="F110" s="119"/>
+      <c r="G110" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H110" s="83">
+      <c r="H110" s="30">
         <v>1</v>
       </c>
-      <c r="I110" s="83" t="s">
+      <c r="I110" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J110" s="30"/>
@@ -5007,23 +5011,23 @@
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A111" s="17"/>
-      <c r="B111" s="107"/>
+      <c r="B111" s="112"/>
       <c r="C111" s="13"/>
       <c r="D111" s="2"/>
-      <c r="E111" s="89"/>
-      <c r="F111" s="96"/>
-      <c r="G111" s="82" t="s">
-        <v>115</v>
-      </c>
-      <c r="H111" s="83">
+      <c r="E111" s="99"/>
+      <c r="F111" s="119"/>
+      <c r="G111" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H111" s="30">
         <v>1</v>
       </c>
-      <c r="I111" s="83" t="s">
+      <c r="I111" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J111" s="30"/>
       <c r="K111" s="31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L111" s="38"/>
       <c r="M111" s="16"/>
@@ -5038,18 +5042,18 @@
     </row>
     <row r="112" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A112" s="17"/>
-      <c r="B112" s="107"/>
+      <c r="B112" s="112"/>
       <c r="C112" s="13"/>
       <c r="D112" s="2"/>
-      <c r="E112" s="89"/>
-      <c r="F112" s="96"/>
-      <c r="G112" s="82" t="s">
+      <c r="E112" s="99"/>
+      <c r="F112" s="119"/>
+      <c r="G112" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H112" s="83">
+      <c r="H112" s="30">
         <v>1</v>
       </c>
-      <c r="I112" s="83" t="s">
+      <c r="I112" s="30" t="s">
         <v>64</v>
       </c>
       <c r="J112" s="30"/>
@@ -5069,18 +5073,18 @@
     </row>
     <row r="113" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A113" s="17"/>
-      <c r="B113" s="107"/>
+      <c r="B113" s="112"/>
       <c r="C113" s="13"/>
       <c r="D113" s="2"/>
-      <c r="E113" s="89"/>
-      <c r="F113" s="96"/>
-      <c r="G113" s="82" t="s">
+      <c r="E113" s="99"/>
+      <c r="F113" s="119"/>
+      <c r="G113" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H113" s="83">
+      <c r="H113" s="30">
         <v>1</v>
       </c>
-      <c r="I113" s="83" t="s">
+      <c r="I113" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J113" s="30"/>
@@ -5100,18 +5104,18 @@
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A114" s="17"/>
-      <c r="B114" s="107"/>
+      <c r="B114" s="112"/>
       <c r="C114" s="13"/>
       <c r="D114" s="2"/>
-      <c r="E114" s="89"/>
-      <c r="F114" s="96"/>
-      <c r="G114" s="82" t="s">
+      <c r="E114" s="99"/>
+      <c r="F114" s="119"/>
+      <c r="G114" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H114" s="123">
+      <c r="H114" s="137">
         <v>2</v>
       </c>
-      <c r="I114" s="123" t="s">
+      <c r="I114" s="137" t="s">
         <v>66</v>
       </c>
       <c r="J114" s="46" t="s">
@@ -5131,18 +5135,18 @@
     </row>
     <row r="115" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A115" s="17"/>
-      <c r="B115" s="107"/>
+      <c r="B115" s="112"/>
       <c r="C115" s="13"/>
       <c r="D115" s="2"/>
-      <c r="E115" s="89"/>
-      <c r="F115" s="96"/>
-      <c r="G115" s="82" t="s">
+      <c r="E115" s="99"/>
+      <c r="F115" s="119"/>
+      <c r="G115" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H115" s="123">
+      <c r="H115" s="137">
         <v>2</v>
       </c>
-      <c r="I115" s="123"/>
+      <c r="I115" s="137"/>
       <c r="J115" s="46"/>
       <c r="K115" s="31"/>
       <c r="L115" s="38"/>
@@ -5156,21 +5160,23 @@
       <c r="T115" s="16"/>
       <c r="U115" s="16"/>
     </row>
-    <row r="116" spans="1:21" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A116" s="17"/>
-      <c r="B116" s="107"/>
+      <c r="B116" s="112"/>
       <c r="C116" s="13"/>
       <c r="D116" s="2"/>
-      <c r="E116" s="89"/>
-      <c r="F116" s="29" t="s">
-        <v>17</v>
-      </c>
+      <c r="E116" s="99"/>
+      <c r="F116" s="119"/>
       <c r="G116" s="82" t="s">
-        <v>17</v>
-      </c>
-      <c r="H116" s="83"/>
-      <c r="I116" s="83"/>
-      <c r="J116" s="30"/>
+        <v>106</v>
+      </c>
+      <c r="H116" s="83">
+        <v>16</v>
+      </c>
+      <c r="I116" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="J116" s="46"/>
       <c r="K116" s="31"/>
       <c r="L116" s="38"/>
       <c r="M116" s="16"/>
@@ -5183,25 +5189,23 @@
       <c r="T116" s="16"/>
       <c r="U116" s="16"/>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A117" s="17"/>
-      <c r="B117" s="107"/>
+      <c r="B117" s="112"/>
       <c r="C117" s="13"/>
       <c r="D117" s="2"/>
-      <c r="E117" s="89"/>
-      <c r="F117" s="96" t="s">
-        <v>68</v>
-      </c>
+      <c r="E117" s="99"/>
+      <c r="F117" s="119"/>
       <c r="G117" s="82" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="H117" s="83">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="I117" s="83" t="s">
-        <v>63</v>
-      </c>
-      <c r="J117" s="30"/>
+        <v>18</v>
+      </c>
+      <c r="J117" s="46"/>
       <c r="K117" s="31"/>
       <c r="L117" s="38"/>
       <c r="M117" s="16"/>
@@ -5214,22 +5218,20 @@
       <c r="T117" s="16"/>
       <c r="U117" s="16"/>
     </row>
-    <row r="118" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:21" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="17"/>
-      <c r="B118" s="107"/>
+      <c r="B118" s="112"/>
       <c r="C118" s="13"/>
       <c r="D118" s="2"/>
-      <c r="E118" s="89"/>
-      <c r="F118" s="96"/>
-      <c r="G118" s="82" t="s">
-        <v>85</v>
-      </c>
-      <c r="H118" s="83">
-        <v>1</v>
-      </c>
-      <c r="I118" s="83" t="s">
-        <v>61</v>
-      </c>
+      <c r="E118" s="99"/>
+      <c r="F118" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G118" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H118" s="30"/>
+      <c r="I118" s="30"/>
       <c r="J118" s="30"/>
       <c r="K118" s="31"/>
       <c r="L118" s="38"/>
@@ -5243,26 +5245,26 @@
       <c r="T118" s="16"/>
       <c r="U118" s="16"/>
     </row>
-    <row r="119" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A119" s="17"/>
-      <c r="B119" s="107"/>
+      <c r="B119" s="112"/>
       <c r="C119" s="13"/>
       <c r="D119" s="2"/>
-      <c r="E119" s="89"/>
-      <c r="F119" s="96"/>
-      <c r="G119" s="82" t="s">
-        <v>115</v>
-      </c>
-      <c r="H119" s="83">
-        <v>1</v>
-      </c>
-      <c r="I119" s="83" t="s">
-        <v>61</v>
+      <c r="E119" s="99"/>
+      <c r="F119" s="119" t="s">
+        <v>68</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H119" s="30">
+        <v>8</v>
+      </c>
+      <c r="I119" s="30" t="s">
+        <v>63</v>
       </c>
       <c r="J119" s="30"/>
-      <c r="K119" s="31" t="s">
-        <v>116</v>
-      </c>
+      <c r="K119" s="31"/>
       <c r="L119" s="38"/>
       <c r="M119" s="16"/>
       <c r="N119" s="16"/>
@@ -5274,27 +5276,25 @@
       <c r="T119" s="16"/>
       <c r="U119" s="16"/>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A120" s="17"/>
-      <c r="B120" s="107"/>
+      <c r="B120" s="112"/>
       <c r="C120" s="13"/>
       <c r="D120" s="2"/>
-      <c r="E120" s="89"/>
-      <c r="F120" s="96"/>
-      <c r="G120" s="82" t="s">
-        <v>59</v>
-      </c>
-      <c r="H120" s="83">
+      <c r="E120" s="99"/>
+      <c r="F120" s="119"/>
+      <c r="G120" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H120" s="30">
         <v>1</v>
       </c>
-      <c r="I120" s="83" t="s">
-        <v>64</v>
+      <c r="I120" s="30" t="s">
+        <v>61</v>
       </c>
       <c r="J120" s="30"/>
       <c r="K120" s="31"/>
-      <c r="L120" s="38" t="s">
-        <v>69</v>
-      </c>
+      <c r="L120" s="38"/>
       <c r="M120" s="16"/>
       <c r="N120" s="16"/>
       <c r="O120" s="16"/>
@@ -5305,25 +5305,25 @@
       <c r="T120" s="16"/>
       <c r="U120" s="16"/>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A121" s="17"/>
-      <c r="B121" s="107"/>
+      <c r="B121" s="112"/>
       <c r="C121" s="13"/>
       <c r="D121" s="2"/>
-      <c r="E121" s="89"/>
-      <c r="F121" s="96"/>
-      <c r="G121" s="82" t="s">
-        <v>60</v>
-      </c>
-      <c r="H121" s="83">
+      <c r="E121" s="99"/>
+      <c r="F121" s="119"/>
+      <c r="G121" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H121" s="30">
         <v>1</v>
       </c>
-      <c r="I121" s="83" t="s">
+      <c r="I121" s="30" t="s">
         <v>61</v>
       </c>
       <c r="J121" s="30"/>
       <c r="K121" s="31" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="L121" s="38"/>
       <c r="M121" s="16"/>
@@ -5336,27 +5336,27 @@
       <c r="T121" s="16"/>
       <c r="U121" s="16"/>
     </row>
-    <row r="122" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A122" s="17"/>
-      <c r="B122" s="107"/>
+      <c r="B122" s="112"/>
       <c r="C122" s="13"/>
       <c r="D122" s="2"/>
-      <c r="E122" s="89"/>
-      <c r="F122" s="96"/>
-      <c r="G122" s="82" t="s">
-        <v>94</v>
-      </c>
-      <c r="H122" s="83">
-        <v>2</v>
-      </c>
-      <c r="I122" s="83" t="s">
-        <v>95</v>
-      </c>
-      <c r="J122" s="30" t="s">
-        <v>96</v>
-      </c>
+      <c r="E122" s="99"/>
+      <c r="F122" s="119"/>
+      <c r="G122" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H122" s="30">
+        <v>1</v>
+      </c>
+      <c r="I122" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="J122" s="30"/>
       <c r="K122" s="31"/>
-      <c r="L122" s="38"/>
+      <c r="L122" s="38" t="s">
+        <v>69</v>
+      </c>
       <c r="M122" s="16"/>
       <c r="N122" s="16"/>
       <c r="O122" s="16"/>
@@ -5367,23 +5367,27 @@
       <c r="T122" s="16"/>
       <c r="U122" s="16"/>
     </row>
-    <row r="123" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A123" s="17"/>
-      <c r="B123" s="107"/>
-      <c r="C123" s="131"/>
-      <c r="D123" s="7"/>
-      <c r="E123" s="95"/>
-      <c r="F123" s="124"/>
-      <c r="G123" s="125" t="s">
-        <v>97</v>
-      </c>
-      <c r="H123" s="126">
-        <v>2</v>
-      </c>
-      <c r="I123" s="126"/>
-      <c r="J123" s="37"/>
-      <c r="K123" s="44"/>
-      <c r="L123" s="132"/>
+      <c r="B123" s="112"/>
+      <c r="C123" s="13"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="99"/>
+      <c r="F123" s="119"/>
+      <c r="G123" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H123" s="30">
+        <v>1</v>
+      </c>
+      <c r="I123" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="J123" s="30"/>
+      <c r="K123" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="L123" s="38"/>
       <c r="M123" s="16"/>
       <c r="N123" s="16"/>
       <c r="O123" s="16"/>
@@ -5394,704 +5398,824 @@
       <c r="T123" s="16"/>
       <c r="U123" s="16"/>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="B124" s="107"/>
-      <c r="L124" s="133"/>
+    <row r="124" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A124" s="17"/>
+      <c r="B124" s="112"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="99"/>
+      <c r="F124" s="119"/>
+      <c r="G124" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H124" s="30">
+        <v>2</v>
+      </c>
+      <c r="I124" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="J124" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="K124" s="31"/>
+      <c r="L124" s="38"/>
+      <c r="M124" s="16"/>
+      <c r="N124" s="16"/>
+      <c r="O124" s="16"/>
+      <c r="P124" s="16"/>
+      <c r="Q124" s="16"/>
+      <c r="R124" s="16"/>
+      <c r="S124" s="16"/>
+      <c r="T124" s="16"/>
+      <c r="U124" s="16"/>
     </row>
     <row r="125" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B125" s="107"/>
-      <c r="H125" s="1"/>
-      <c r="I125" s="1"/>
-      <c r="J125" s="1"/>
-      <c r="K125" s="1"/>
-      <c r="L125" s="133"/>
+      <c r="A125" s="17"/>
+      <c r="B125" s="112"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="99"/>
+      <c r="F125" s="119"/>
+      <c r="G125" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H125" s="30">
+        <v>2</v>
+      </c>
+      <c r="I125" s="30"/>
+      <c r="J125" s="30"/>
+      <c r="K125" s="31"/>
+      <c r="L125" s="38"/>
+      <c r="M125" s="16"/>
+      <c r="N125" s="16"/>
+      <c r="O125" s="16"/>
+      <c r="P125" s="16"/>
+      <c r="Q125" s="16"/>
+      <c r="R125" s="16"/>
+      <c r="S125" s="16"/>
+      <c r="T125" s="16"/>
+      <c r="U125" s="16"/>
     </row>
     <row r="126" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B126" s="107"/>
-      <c r="C126" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="D126" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="E126" s="128" t="s">
+      <c r="A126" s="17"/>
+      <c r="B126" s="112"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="2"/>
+      <c r="E126" s="99"/>
+      <c r="F126" s="119"/>
+      <c r="G126" s="82" t="s">
+        <v>106</v>
+      </c>
+      <c r="H126" s="83">
+        <v>16</v>
+      </c>
+      <c r="I126" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="J126" s="30"/>
+      <c r="K126" s="31"/>
+      <c r="L126" s="38"/>
+      <c r="M126" s="16"/>
+      <c r="N126" s="16"/>
+      <c r="O126" s="16"/>
+      <c r="P126" s="16"/>
+      <c r="Q126" s="16"/>
+      <c r="R126" s="16"/>
+      <c r="S126" s="16"/>
+      <c r="T126" s="16"/>
+      <c r="U126" s="16"/>
+    </row>
+    <row r="127" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="17"/>
+      <c r="B127" s="112"/>
+      <c r="C127" s="90"/>
+      <c r="D127" s="7"/>
+      <c r="E127" s="103"/>
+      <c r="F127" s="120"/>
+      <c r="G127" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="H127" s="85">
+        <v>32</v>
+      </c>
+      <c r="I127" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="J127" s="37"/>
+      <c r="K127" s="44"/>
+      <c r="L127" s="91"/>
+      <c r="M127" s="16"/>
+      <c r="N127" s="16"/>
+      <c r="O127" s="16"/>
+      <c r="P127" s="16"/>
+      <c r="Q127" s="16"/>
+      <c r="R127" s="16"/>
+      <c r="S127" s="16"/>
+      <c r="T127" s="16"/>
+      <c r="U127" s="16"/>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="B128" s="112"/>
+      <c r="L128" s="92"/>
+    </row>
+    <row r="129" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B129" s="112"/>
+      <c r="G129" s="138"/>
+      <c r="H129" s="136"/>
+      <c r="I129" s="136"/>
+      <c r="J129" s="1"/>
+      <c r="K129" s="1"/>
+      <c r="L129" s="92"/>
+    </row>
+    <row r="130" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B130" s="112"/>
+      <c r="C130" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="D130" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E130" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="F126" s="98" t="s">
+      <c r="F130" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="G126" s="39" t="s">
+      <c r="G130" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="H126" s="40">
+      <c r="H130" s="40">
         <v>2</v>
       </c>
-      <c r="I126" s="40"/>
-      <c r="J126" s="40"/>
-      <c r="K126" s="41"/>
-      <c r="L126" s="133"/>
-    </row>
-    <row r="127" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B127" s="107"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="11"/>
-      <c r="E127" s="120"/>
-      <c r="F127" s="99"/>
-      <c r="G127" s="6" t="s">
+      <c r="I130" s="40"/>
+      <c r="J130" s="40"/>
+      <c r="K130" s="41"/>
+      <c r="L130" s="92"/>
+    </row>
+    <row r="131" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B131" s="112"/>
+      <c r="C131" s="2"/>
+      <c r="D131" s="11"/>
+      <c r="E131" s="104"/>
+      <c r="F131" s="107"/>
+      <c r="G131" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H127" s="30">
+      <c r="H131" s="30">
         <v>1</v>
       </c>
-      <c r="I127" s="30"/>
-      <c r="J127" s="30"/>
-      <c r="K127" s="31"/>
-      <c r="L127" s="133"/>
-    </row>
-    <row r="128" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B128" s="107"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="120"/>
-      <c r="F128" s="100"/>
-      <c r="G128" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H128" s="42">
-        <v>1</v>
-      </c>
-      <c r="I128" s="42"/>
-      <c r="J128" s="42"/>
-      <c r="K128" s="43"/>
-      <c r="L128" s="133"/>
-    </row>
-    <row r="129" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B129" s="107"/>
-      <c r="C129" s="2"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="120"/>
-      <c r="F129" s="29"/>
-      <c r="G129" s="82" t="s">
-        <v>109</v>
-      </c>
-      <c r="H129" s="83">
-        <v>8</v>
-      </c>
-      <c r="I129" s="83" t="s">
-        <v>122</v>
-      </c>
-      <c r="J129" s="30"/>
-      <c r="K129" s="31"/>
-      <c r="L129" s="133"/>
-    </row>
-    <row r="130" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B130" s="107"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="129"/>
-      <c r="F130" s="3"/>
-      <c r="G130" s="127" t="s">
-        <v>120</v>
-      </c>
-      <c r="H130" s="136">
-        <v>16</v>
-      </c>
-      <c r="I130" s="136" t="s">
-        <v>123</v>
-      </c>
-      <c r="J130" s="42"/>
-      <c r="K130" s="43"/>
-      <c r="L130" s="133" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="131" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B131" s="107"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
-      <c r="E131" s="75"/>
-      <c r="F131" s="2"/>
-      <c r="G131" s="6"/>
-      <c r="H131" s="30"/>
       <c r="I131" s="30"/>
       <c r="J131" s="30"/>
       <c r="K131" s="31"/>
-      <c r="L131" s="133"/>
+      <c r="L131" s="92"/>
     </row>
     <row r="132" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B132" s="107"/>
+      <c r="B132" s="112"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
-      <c r="E132" s="94" t="s">
-        <v>12</v>
-      </c>
-      <c r="F132" s="91" t="s">
-        <v>5</v>
-      </c>
-      <c r="G132" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="H132" s="40">
-        <v>2</v>
-      </c>
-      <c r="I132" s="40"/>
-      <c r="J132" s="40"/>
-      <c r="K132" s="41"/>
-      <c r="L132" s="133"/>
+      <c r="E132" s="104"/>
+      <c r="F132" s="108"/>
+      <c r="G132" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H132" s="42">
+        <v>1</v>
+      </c>
+      <c r="I132" s="42"/>
+      <c r="J132" s="42"/>
+      <c r="K132" s="43"/>
+      <c r="L132" s="92"/>
     </row>
     <row r="133" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B133" s="107"/>
+      <c r="B133" s="112"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
-      <c r="E133" s="89"/>
-      <c r="F133" s="92"/>
+      <c r="E133" s="104"/>
+      <c r="F133" s="29"/>
       <c r="G133" s="6" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
       <c r="H133" s="30">
-        <v>1</v>
-      </c>
-      <c r="I133" s="30"/>
+        <v>8</v>
+      </c>
+      <c r="I133" s="30" t="s">
+        <v>120</v>
+      </c>
       <c r="J133" s="30"/>
       <c r="K133" s="31"/>
-      <c r="L133" s="133"/>
+      <c r="L133" s="92"/>
     </row>
     <row r="134" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B134" s="107"/>
+      <c r="B134" s="112"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
-      <c r="E134" s="89"/>
-      <c r="F134" s="93"/>
+      <c r="E134" s="110"/>
+      <c r="F134" s="3"/>
       <c r="G134" s="14" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
       <c r="H134" s="42">
-        <v>1</v>
-      </c>
-      <c r="I134" s="42"/>
+        <v>16</v>
+      </c>
+      <c r="I134" s="42" t="s">
+        <v>121</v>
+      </c>
       <c r="J134" s="42"/>
       <c r="K134" s="43"/>
-      <c r="L134" s="133"/>
+      <c r="L134" s="92" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="135" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B135" s="107"/>
+      <c r="B135" s="112"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
-      <c r="E135" s="89"/>
+      <c r="E135" s="75"/>
       <c r="F135" s="2"/>
-      <c r="G135" s="82" t="s">
-        <v>109</v>
-      </c>
-      <c r="H135" s="83">
-        <v>8</v>
-      </c>
-      <c r="I135" s="83" t="s">
-        <v>121</v>
-      </c>
+      <c r="G135" s="6"/>
+      <c r="H135" s="30"/>
+      <c r="I135" s="30"/>
       <c r="J135" s="30"/>
       <c r="K135" s="31"/>
-      <c r="L135" s="133"/>
-    </row>
-    <row r="136" spans="2:12" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B136" s="107"/>
-      <c r="C136" s="7"/>
-      <c r="D136" s="7"/>
-      <c r="E136" s="95"/>
-      <c r="F136" s="7"/>
-      <c r="G136" s="125" t="s">
-        <v>120</v>
-      </c>
-      <c r="H136" s="137">
+      <c r="L135" s="92"/>
+    </row>
+    <row r="136" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B136" s="112"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="F136" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="G136" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H136" s="40">
+        <v>2</v>
+      </c>
+      <c r="I136" s="40"/>
+      <c r="J136" s="40"/>
+      <c r="K136" s="41"/>
+      <c r="L136" s="92"/>
+    </row>
+    <row r="137" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B137" s="112"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2"/>
+      <c r="E137" s="99"/>
+      <c r="F137" s="101"/>
+      <c r="G137" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H137" s="30">
+        <v>1</v>
+      </c>
+      <c r="I137" s="30"/>
+      <c r="J137" s="30"/>
+      <c r="K137" s="31"/>
+      <c r="L137" s="92"/>
+    </row>
+    <row r="138" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B138" s="112"/>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="99"/>
+      <c r="F138" s="102"/>
+      <c r="G138" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H138" s="42">
+        <v>1</v>
+      </c>
+      <c r="I138" s="42"/>
+      <c r="J138" s="42"/>
+      <c r="K138" s="43"/>
+      <c r="L138" s="92"/>
+    </row>
+    <row r="139" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B139" s="112"/>
+      <c r="C139" s="2"/>
+      <c r="D139" s="2"/>
+      <c r="E139" s="99"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H139" s="30">
+        <v>8</v>
+      </c>
+      <c r="I139" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="J139" s="30"/>
+      <c r="K139" s="31"/>
+      <c r="L139" s="92"/>
+    </row>
+    <row r="140" spans="2:12" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B140" s="112"/>
+      <c r="C140" s="7"/>
+      <c r="D140" s="7"/>
+      <c r="E140" s="103"/>
+      <c r="F140" s="7"/>
+      <c r="G140" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="H140" s="37">
         <v>16</v>
       </c>
-      <c r="I136" s="137" t="s">
+      <c r="I140" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="J140" s="37"/>
+      <c r="K140" s="44"/>
+      <c r="L140" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="J136" s="37"/>
-      <c r="K136" s="44"/>
-      <c r="L136" s="134" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="137" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B137" s="107"/>
-      <c r="H137" s="1"/>
-      <c r="I137" s="1"/>
-      <c r="J137" s="1"/>
-      <c r="K137" s="1"/>
-      <c r="L137" s="133"/>
-    </row>
-    <row r="138" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B138" s="107"/>
-      <c r="H138" s="1"/>
-      <c r="I138" s="1"/>
-      <c r="J138" s="1"/>
-      <c r="K138" s="1"/>
-      <c r="L138" s="133"/>
-    </row>
-    <row r="139" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B139" s="107"/>
-      <c r="C139" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="D139" s="36" t="s">
+    </row>
+    <row r="141" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B141" s="112"/>
+      <c r="G141" s="138"/>
+      <c r="H141" s="136"/>
+      <c r="I141" s="136"/>
+      <c r="J141" s="1"/>
+      <c r="K141" s="1"/>
+      <c r="L141" s="92"/>
+    </row>
+    <row r="142" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B142" s="112"/>
+      <c r="G142" s="138"/>
+      <c r="H142" s="136"/>
+      <c r="I142" s="136"/>
+      <c r="J142" s="1"/>
+      <c r="K142" s="1"/>
+      <c r="L142" s="92"/>
+    </row>
+    <row r="143" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B143" s="112"/>
+      <c r="C143" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="E139" s="128" t="s">
+      <c r="D143" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="E143" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="F139" s="98" t="s">
+      <c r="F143" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="G139" s="39" t="s">
+      <c r="G143" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="H139" s="40">
+      <c r="H143" s="40">
         <v>2</v>
       </c>
-      <c r="I139" s="40"/>
-      <c r="J139" s="40"/>
-      <c r="K139" s="41"/>
-      <c r="L139" s="133"/>
-    </row>
-    <row r="140" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B140" s="107"/>
-      <c r="C140" s="2"/>
-      <c r="D140" s="11"/>
-      <c r="E140" s="120"/>
-      <c r="F140" s="99"/>
-      <c r="G140" s="6" t="s">
+      <c r="I143" s="40"/>
+      <c r="J143" s="40"/>
+      <c r="K143" s="41"/>
+      <c r="L143" s="92"/>
+    </row>
+    <row r="144" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B144" s="112"/>
+      <c r="C144" s="2"/>
+      <c r="D144" s="11"/>
+      <c r="E144" s="104"/>
+      <c r="F144" s="107"/>
+      <c r="G144" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H140" s="30">
+      <c r="H144" s="30">
         <v>1</v>
       </c>
-      <c r="I140" s="30"/>
-      <c r="J140" s="30"/>
-      <c r="K140" s="31"/>
-      <c r="L140" s="133"/>
-    </row>
-    <row r="141" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B141" s="107"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
-      <c r="E141" s="120"/>
-      <c r="F141" s="100"/>
-      <c r="G141" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H141" s="42">
-        <v>1</v>
-      </c>
-      <c r="I141" s="42"/>
-      <c r="J141" s="42"/>
-      <c r="K141" s="43"/>
-      <c r="L141" s="133"/>
-    </row>
-    <row r="142" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B142" s="107"/>
-      <c r="C142" s="2"/>
-      <c r="D142" s="2"/>
-      <c r="E142" s="120"/>
-      <c r="F142" s="29"/>
-      <c r="G142" s="82" t="s">
-        <v>138</v>
-      </c>
-      <c r="H142" s="83">
-        <v>32</v>
-      </c>
-      <c r="I142" s="83" t="s">
-        <v>104</v>
-      </c>
-      <c r="J142" s="30"/>
-      <c r="K142" s="31"/>
-      <c r="L142" s="133"/>
-    </row>
-    <row r="143" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B143" s="107"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="129"/>
-      <c r="F143" s="3"/>
-      <c r="G143" s="127" t="s">
-        <v>139</v>
-      </c>
-      <c r="H143" s="136">
-        <v>16</v>
-      </c>
-      <c r="I143" s="136" t="s">
-        <v>123</v>
-      </c>
-      <c r="J143" s="42"/>
-      <c r="K143" s="43"/>
-      <c r="L143" s="133" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="144" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B144" s="107"/>
-      <c r="C144" s="2"/>
-      <c r="D144" s="2"/>
-      <c r="E144" s="75"/>
-      <c r="F144" s="2"/>
-      <c r="G144" s="6"/>
-      <c r="H144" s="30"/>
       <c r="I144" s="30"/>
       <c r="J144" s="30"/>
       <c r="K144" s="31"/>
-      <c r="L144" s="133"/>
+      <c r="L144" s="92"/>
     </row>
     <row r="145" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B145" s="107"/>
+      <c r="B145" s="112"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
-      <c r="E145" s="94" t="s">
-        <v>12</v>
-      </c>
-      <c r="F145" s="91" t="s">
-        <v>5</v>
-      </c>
-      <c r="G145" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="H145" s="40">
-        <v>2</v>
-      </c>
-      <c r="I145" s="40"/>
-      <c r="J145" s="40"/>
-      <c r="K145" s="41"/>
-      <c r="L145" s="133"/>
+      <c r="E145" s="104"/>
+      <c r="F145" s="108"/>
+      <c r="G145" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H145" s="42">
+        <v>1</v>
+      </c>
+      <c r="I145" s="42"/>
+      <c r="J145" s="42"/>
+      <c r="K145" s="43"/>
+      <c r="L145" s="92"/>
     </row>
     <row r="146" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B146" s="107"/>
+      <c r="B146" s="112"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
-      <c r="E146" s="89"/>
-      <c r="F146" s="92"/>
+      <c r="E146" s="104"/>
+      <c r="F146" s="29"/>
       <c r="G146" s="6" t="s">
-        <v>26</v>
+        <v>136</v>
       </c>
       <c r="H146" s="30">
-        <v>1</v>
-      </c>
-      <c r="I146" s="30"/>
+        <v>32</v>
+      </c>
+      <c r="I146" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="J146" s="30"/>
       <c r="K146" s="31"/>
-      <c r="L146" s="133"/>
+      <c r="L146" s="92"/>
     </row>
     <row r="147" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B147" s="107"/>
+      <c r="B147" s="112"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
-      <c r="E147" s="89"/>
-      <c r="F147" s="93"/>
+      <c r="E147" s="110"/>
+      <c r="F147" s="3"/>
       <c r="G147" s="14" t="s">
-        <v>24</v>
+        <v>137</v>
       </c>
       <c r="H147" s="42">
-        <v>1</v>
-      </c>
-      <c r="I147" s="42"/>
+        <v>16</v>
+      </c>
+      <c r="I147" s="42" t="s">
+        <v>121</v>
+      </c>
       <c r="J147" s="42"/>
       <c r="K147" s="43"/>
-      <c r="L147" s="133"/>
-    </row>
-    <row r="148" spans="1:12" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B148" s="107"/>
-      <c r="C148" s="7"/>
-      <c r="D148" s="7"/>
-      <c r="E148" s="95"/>
-      <c r="F148" s="7"/>
-      <c r="G148" s="8"/>
-      <c r="H148" s="37"/>
-      <c r="I148" s="37"/>
-      <c r="J148" s="37"/>
-      <c r="K148" s="44"/>
-      <c r="L148" s="134"/>
+      <c r="L147" s="92" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B148" s="112"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+      <c r="E148" s="75"/>
+      <c r="F148" s="2"/>
+      <c r="G148" s="6"/>
+      <c r="H148" s="30"/>
+      <c r="I148" s="30"/>
+      <c r="J148" s="30"/>
+      <c r="K148" s="31"/>
+      <c r="L148" s="92"/>
     </row>
     <row r="149" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B149" s="107"/>
-      <c r="H149" s="1"/>
-      <c r="I149" s="1"/>
-      <c r="J149" s="1"/>
-      <c r="K149" s="1"/>
-      <c r="L149" s="133"/>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A150" s="1"/>
-      <c r="B150" s="107"/>
-      <c r="C150" s="1"/>
-      <c r="D150" s="1"/>
-      <c r="E150" s="1"/>
-      <c r="F150" s="1"/>
-      <c r="G150" s="1"/>
-      <c r="L150" s="133"/>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A151" s="1"/>
-      <c r="B151" s="107"/>
-      <c r="C151" s="34" t="s">
+      <c r="B149" s="112"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+      <c r="E149" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="F149" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="G149" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H149" s="40">
+        <v>2</v>
+      </c>
+      <c r="I149" s="40"/>
+      <c r="J149" s="40"/>
+      <c r="K149" s="41"/>
+      <c r="L149" s="92"/>
+    </row>
+    <row r="150" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B150" s="112"/>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
+      <c r="E150" s="99"/>
+      <c r="F150" s="101"/>
+      <c r="G150" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H150" s="30">
+        <v>1</v>
+      </c>
+      <c r="I150" s="30"/>
+      <c r="J150" s="30"/>
+      <c r="K150" s="31"/>
+      <c r="L150" s="92"/>
+    </row>
+    <row r="151" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B151" s="112"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
+      <c r="E151" s="99"/>
+      <c r="F151" s="102"/>
+      <c r="G151" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H151" s="42">
+        <v>1</v>
+      </c>
+      <c r="I151" s="42"/>
+      <c r="J151" s="42"/>
+      <c r="K151" s="43"/>
+      <c r="L151" s="92"/>
+    </row>
+    <row r="152" spans="1:12" s="15" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B152" s="112"/>
+      <c r="C152" s="7"/>
+      <c r="D152" s="7"/>
+      <c r="E152" s="103"/>
+      <c r="F152" s="7"/>
+      <c r="G152" s="8"/>
+      <c r="H152" s="37"/>
+      <c r="I152" s="37"/>
+      <c r="J152" s="37"/>
+      <c r="K152" s="44"/>
+      <c r="L152" s="93"/>
+    </row>
+    <row r="153" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B153" s="112"/>
+      <c r="G153" s="138"/>
+      <c r="H153" s="136"/>
+      <c r="I153" s="136"/>
+      <c r="J153" s="1"/>
+      <c r="K153" s="1"/>
+      <c r="L153" s="92"/>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A154" s="1"/>
+      <c r="B154" s="112"/>
+      <c r="C154" s="1"/>
+      <c r="D154" s="1"/>
+      <c r="E154" s="1"/>
+      <c r="F154" s="1"/>
+      <c r="G154" s="136"/>
+      <c r="L154" s="92"/>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A155" s="1"/>
+      <c r="B155" s="112"/>
+      <c r="C155" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D151" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="E151" s="108" t="s">
+      <c r="D155" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="E155" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="F151" s="113" t="s">
+      <c r="F155" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="G151" s="63" t="s">
+      <c r="G155" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="H151" s="64">
+      <c r="H155" s="64">
         <v>2</v>
       </c>
-      <c r="I151" s="64"/>
-      <c r="J151" s="64"/>
-      <c r="K151" s="65"/>
-      <c r="L151" s="76"/>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A152" s="1"/>
-      <c r="B152" s="107"/>
-      <c r="C152" s="2"/>
-      <c r="D152" s="11"/>
-      <c r="E152" s="109"/>
-      <c r="F152" s="114"/>
-      <c r="G152" s="6" t="s">
+      <c r="I155" s="64"/>
+      <c r="J155" s="64"/>
+      <c r="K155" s="65"/>
+      <c r="L155" s="76"/>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A156" s="1"/>
+      <c r="B156" s="112"/>
+      <c r="C156" s="2"/>
+      <c r="D156" s="11"/>
+      <c r="E156" s="114"/>
+      <c r="F156" s="122"/>
+      <c r="G156" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H152" s="30">
+      <c r="H156" s="30">
         <v>1</v>
       </c>
-      <c r="I152" s="30"/>
-      <c r="J152" s="30"/>
-      <c r="K152" s="66"/>
-      <c r="L152" s="38"/>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A153" s="1"/>
-      <c r="B153" s="107"/>
-      <c r="C153" s="2"/>
-      <c r="D153" s="2"/>
-      <c r="E153" s="109"/>
-      <c r="F153" s="115"/>
-      <c r="G153" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H153" s="42">
-        <v>1</v>
-      </c>
-      <c r="I153" s="42"/>
-      <c r="J153" s="42"/>
-      <c r="K153" s="77"/>
-      <c r="L153" s="38"/>
-    </row>
-    <row r="154" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="1"/>
-      <c r="B154" s="107"/>
-      <c r="C154" s="2"/>
-      <c r="D154" s="2"/>
-      <c r="E154" s="109"/>
-      <c r="F154" s="118"/>
-      <c r="G154" s="82" t="s">
-        <v>100</v>
-      </c>
-      <c r="H154" s="83">
-        <v>1</v>
-      </c>
-      <c r="I154" s="83" t="s">
-        <v>101</v>
-      </c>
-      <c r="J154" s="30"/>
-      <c r="K154" s="66"/>
-      <c r="L154" s="38" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="155" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="1"/>
-      <c r="B155" s="107"/>
-      <c r="C155" s="2"/>
-      <c r="D155" s="2"/>
-      <c r="E155" s="109"/>
-      <c r="F155" s="118"/>
-      <c r="G155" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="H155" s="83">
-        <v>3</v>
-      </c>
-      <c r="I155" s="83"/>
-      <c r="J155" s="30"/>
-      <c r="K155" s="66"/>
-      <c r="L155" s="38"/>
-    </row>
-    <row r="156" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="1"/>
-      <c r="B156" s="107"/>
-      <c r="C156" s="2"/>
-      <c r="D156" s="2"/>
-      <c r="E156" s="109"/>
-      <c r="F156" s="78"/>
-      <c r="G156" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H156" s="30">
-        <v>4</v>
-      </c>
-      <c r="I156" s="30" t="s">
-        <v>62</v>
-      </c>
+      <c r="I156" s="30"/>
       <c r="J156" s="30"/>
       <c r="K156" s="66"/>
       <c r="L156" s="38"/>
     </row>
-    <row r="157" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A157" s="1"/>
-      <c r="B157" s="107"/>
+      <c r="B157" s="112"/>
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
-      <c r="E157" s="110"/>
-      <c r="F157" s="79"/>
-      <c r="G157" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="H157" s="68">
-        <v>16</v>
-      </c>
-      <c r="I157" s="68" t="s">
-        <v>53</v>
-      </c>
-      <c r="J157" s="68"/>
-      <c r="K157" s="69"/>
+      <c r="E157" s="114"/>
+      <c r="F157" s="123"/>
+      <c r="G157" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H157" s="42">
+        <v>1</v>
+      </c>
+      <c r="I157" s="42"/>
+      <c r="J157" s="42"/>
+      <c r="K157" s="77"/>
       <c r="L157" s="38"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A158" s="1"/>
-      <c r="B158" s="107"/>
+      <c r="B158" s="112"/>
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
-      <c r="E158" s="75"/>
-      <c r="F158" s="2"/>
-      <c r="G158" s="6"/>
-      <c r="H158" s="30"/>
-      <c r="I158" s="30"/>
+      <c r="E158" s="114"/>
+      <c r="F158" s="87"/>
+      <c r="G158" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H158" s="30">
+        <v>1</v>
+      </c>
+      <c r="I158" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="J158" s="30"/>
-      <c r="K158" s="31"/>
-      <c r="L158" s="32"/>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K158" s="66"/>
+      <c r="L158" s="38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A159" s="1"/>
-      <c r="B159" s="107"/>
+      <c r="B159" s="112"/>
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
-      <c r="E159" s="105" t="s">
-        <v>12</v>
-      </c>
-      <c r="F159" s="116" t="s">
-        <v>5</v>
-      </c>
-      <c r="G159" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="H159" s="40">
-        <v>2</v>
-      </c>
-      <c r="I159" s="40"/>
-      <c r="J159" s="40"/>
-      <c r="K159" s="41"/>
+      <c r="E159" s="114"/>
+      <c r="F159" s="87"/>
+      <c r="G159" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H159" s="30">
+        <v>3</v>
+      </c>
+      <c r="I159" s="30"/>
+      <c r="J159" s="30"/>
+      <c r="K159" s="66"/>
       <c r="L159" s="38"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A160" s="1"/>
-      <c r="B160" s="107"/>
+      <c r="B160" s="112"/>
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
-      <c r="E160" s="89"/>
-      <c r="F160" s="99"/>
+      <c r="E160" s="114"/>
+      <c r="F160" s="78"/>
       <c r="G160" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H160" s="30">
+        <v>4</v>
+      </c>
+      <c r="I160" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="J160" s="30"/>
+      <c r="K160" s="66"/>
+      <c r="L160" s="38"/>
+    </row>
+    <row r="161" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A161" s="1"/>
+      <c r="B161" s="112"/>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="115"/>
+      <c r="F161" s="79"/>
+      <c r="G161" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="H161" s="68">
+        <v>16</v>
+      </c>
+      <c r="I161" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="J161" s="68"/>
+      <c r="K161" s="69"/>
+      <c r="L161" s="38"/>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A162" s="1"/>
+      <c r="B162" s="112"/>
+      <c r="C162" s="2"/>
+      <c r="D162" s="2"/>
+      <c r="E162" s="75"/>
+      <c r="F162" s="2"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="30"/>
+      <c r="I162" s="30"/>
+      <c r="J162" s="30"/>
+      <c r="K162" s="31"/>
+      <c r="L162" s="32"/>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A163" s="1"/>
+      <c r="B163" s="112"/>
+      <c r="C163" s="2"/>
+      <c r="D163" s="2"/>
+      <c r="E163" s="124" t="s">
+        <v>12</v>
+      </c>
+      <c r="F163" s="126" t="s">
+        <v>5</v>
+      </c>
+      <c r="G163" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H163" s="40">
+        <v>2</v>
+      </c>
+      <c r="I163" s="40"/>
+      <c r="J163" s="40"/>
+      <c r="K163" s="41"/>
+      <c r="L163" s="38"/>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A164" s="1"/>
+      <c r="B164" s="112"/>
+      <c r="C164" s="2"/>
+      <c r="D164" s="2"/>
+      <c r="E164" s="99"/>
+      <c r="F164" s="107"/>
+      <c r="G164" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H160" s="30">
+      <c r="H164" s="30">
         <v>1</v>
       </c>
-      <c r="I160" s="30"/>
-      <c r="J160" s="30"/>
-      <c r="K160" s="31"/>
-      <c r="L160" s="38"/>
-    </row>
-    <row r="161" spans="1:12" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="1"/>
-      <c r="B161" s="107"/>
-      <c r="C161" s="72"/>
-      <c r="D161" s="80"/>
-      <c r="E161" s="90"/>
-      <c r="F161" s="117"/>
-      <c r="G161" s="61" t="s">
+      <c r="I164" s="30"/>
+      <c r="J164" s="30"/>
+      <c r="K164" s="31"/>
+      <c r="L164" s="38"/>
+    </row>
+    <row r="165" spans="1:12" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="1"/>
+      <c r="B165" s="112"/>
+      <c r="C165" s="72"/>
+      <c r="D165" s="80"/>
+      <c r="E165" s="125"/>
+      <c r="F165" s="127"/>
+      <c r="G165" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="H161" s="62">
+      <c r="H165" s="62">
         <v>1</v>
       </c>
-      <c r="I161" s="62"/>
-      <c r="J161" s="62"/>
-      <c r="K161" s="73"/>
-      <c r="L161" s="74"/>
+      <c r="I165" s="62"/>
+      <c r="J165" s="62"/>
+      <c r="K165" s="73"/>
+      <c r="L165" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="E9:E16"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="E104:E127"/>
+    <mergeCell ref="F104:F106"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E34:E44"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="E64:E81"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="F109:F117"/>
+    <mergeCell ref="F163:F165"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="E149:E152"/>
+    <mergeCell ref="F149:F151"/>
+    <mergeCell ref="F69:F74"/>
+    <mergeCell ref="F76:F81"/>
+    <mergeCell ref="B4:B165"/>
+    <mergeCell ref="E155:E161"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="E51:E57"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="F107:F108"/>
+    <mergeCell ref="F119:F127"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="F155:F157"/>
+    <mergeCell ref="E163:E165"/>
+    <mergeCell ref="F130:F132"/>
+    <mergeCell ref="E136:E140"/>
+    <mergeCell ref="F136:F138"/>
+    <mergeCell ref="E130:E134"/>
+    <mergeCell ref="E143:E147"/>
+    <mergeCell ref="F143:F145"/>
     <mergeCell ref="E84:E86"/>
     <mergeCell ref="F84:F86"/>
     <mergeCell ref="E88:E97"/>
     <mergeCell ref="F88:F90"/>
     <mergeCell ref="F93:F94"/>
     <mergeCell ref="F96:F97"/>
-    <mergeCell ref="F126:F128"/>
-    <mergeCell ref="E132:E136"/>
-    <mergeCell ref="F132:F134"/>
-    <mergeCell ref="E126:E130"/>
-    <mergeCell ref="E139:E143"/>
-    <mergeCell ref="F139:F141"/>
-    <mergeCell ref="E145:E148"/>
-    <mergeCell ref="F145:F147"/>
-    <mergeCell ref="F69:F74"/>
-    <mergeCell ref="F76:F81"/>
-    <mergeCell ref="B4:B161"/>
-    <mergeCell ref="E151:E157"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="E51:E57"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="F107:F108"/>
-    <mergeCell ref="F117:F123"/>
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="F151:F153"/>
-    <mergeCell ref="E159:E161"/>
-    <mergeCell ref="F159:F161"/>
-    <mergeCell ref="F100:F102"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="E9:E16"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="E104:E123"/>
-    <mergeCell ref="F104:F106"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="E34:E44"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="F109:F115"/>
-    <mergeCell ref="E60:E62"/>
-    <mergeCell ref="F60:F62"/>
-    <mergeCell ref="E64:E81"/>
-    <mergeCell ref="F64:F66"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6101,10 +6225,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6117,7 +6241,7 @@
       <c r="A1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="86" t="s">
         <v>88</v>
       </c>
       <c r="C1" s="15" t="s">
@@ -6128,7 +6252,7 @@
       <c r="A2" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="86" t="s">
         <v>92</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -6137,13 +6261,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3">
         <v>1.1000000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4">
+        <v>1.2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>